<commit_message>
almost donde with the timeline page
</commit_message>
<xml_diff>
--- a/src/recursos/BDD Timeline.xlsx
+++ b/src/recursos/BDD Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Files\Programming\portfolio\src\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294C76C0-F56D-49BB-A336-75D84AE1AB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D635B61E-6C20-4C68-8732-BE127092AB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
   </bookViews>
@@ -625,12 +625,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -646,13 +652,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -971,7 +978,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:XFD43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -997,28 +1006,28 @@
       <c r="A1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="6" t="s">
         <v>80</v>
       </c>
       <c r="J1" t="s">
@@ -1080,7 +1089,7 @@
         <v>"image":"https://i.postimg.cc/BvVNXsLg/ARREL.png"</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="L2:S17" si="1">CONCATENATE(C$1,$M$1,C2)</f>
+        <f t="shared" ref="M2:Q17" si="1">CONCATENATE(C$1,$M$1,C2)</f>
         <v>"category":"Work"</v>
       </c>
       <c r="N2" t="str">
@@ -2187,23 +2196,23 @@
         <v>"image":"https://i.postimg.cc/FHhT6TXj/APICS.png"</v>
       </c>
       <c r="M18" t="str">
-        <f>CONCATENATE(C$1,$M$1,C18)</f>
+        <f t="shared" ref="M18:Q23" si="6">CONCATENATE(C$1,$M$1,C18)</f>
         <v>"category":"Education"</v>
       </c>
       <c r="N18" t="str">
-        <f>CONCATENATE(D$1,$M$1,D18)</f>
+        <f t="shared" si="6"/>
         <v>"name":"Inventory control"</v>
       </c>
       <c r="O18" t="str">
-        <f>CONCATENATE(E$1,$M$1,E18)</f>
+        <f t="shared" si="6"/>
         <v>"location":"EDOMEX"</v>
       </c>
       <c r="P18" t="str">
-        <f>CONCATENATE(F$1,$M$1,F18)</f>
+        <f t="shared" si="6"/>
         <v>"businessName":"APICs"</v>
       </c>
       <c r="Q18" t="str">
-        <f>CONCATENATE(G$1,$M$1,G18)</f>
+        <f t="shared" si="6"/>
         <v>"description":"reorder point, costs, ABC classification"</v>
       </c>
       <c r="R18" t="str">
@@ -2256,23 +2265,23 @@
         <v>"image":"https://i.postimg.cc/FHhT6TXj/APICS.png"</v>
       </c>
       <c r="M19" t="str">
-        <f>CONCATENATE(C$1,$M$1,C19)</f>
+        <f t="shared" si="6"/>
         <v>"category":"Education"</v>
       </c>
       <c r="N19" t="str">
-        <f>CONCATENATE(D$1,$M$1,D19)</f>
+        <f t="shared" si="6"/>
         <v>"name":"Procurement planning"</v>
       </c>
       <c r="O19" t="str">
-        <f>CONCATENATE(E$1,$M$1,E19)</f>
+        <f t="shared" si="6"/>
         <v>"location":"EDOMEX"</v>
       </c>
       <c r="P19" t="str">
-        <f>CONCATENATE(F$1,$M$1,F19)</f>
+        <f t="shared" si="6"/>
         <v>"businessName":"APICs"</v>
       </c>
       <c r="Q19" t="str">
-        <f>CONCATENATE(G$1,$M$1,G19)</f>
+        <f t="shared" si="6"/>
         <v>"description":"sourcing, supplier management, OOS, CSL"</v>
       </c>
       <c r="R19" t="str">
@@ -2325,23 +2334,23 @@
         <v>"image":"https://i.postimg.cc/KYRDXVqg/ITESM.png"</v>
       </c>
       <c r="M20" t="str">
-        <f>CONCATENATE(C$1,$M$1,C20)</f>
+        <f t="shared" si="6"/>
         <v>"category":"Education"</v>
       </c>
       <c r="N20" t="str">
-        <f>CONCATENATE(D$1,$M$1,D20)</f>
+        <f t="shared" si="6"/>
         <v>"name":"Six Sigma"</v>
       </c>
       <c r="O20" t="str">
-        <f>CONCATENATE(E$1,$M$1,E20)</f>
+        <f t="shared" si="6"/>
         <v>"location":"CDMX"</v>
       </c>
       <c r="P20" t="str">
-        <f>CONCATENATE(F$1,$M$1,F20)</f>
+        <f t="shared" si="6"/>
         <v>"businessName":"ITESM"</v>
       </c>
       <c r="Q20" t="str">
-        <f>CONCATENATE(G$1,$M$1,G20)</f>
+        <f t="shared" si="6"/>
         <v>"description":"DMAIC methodology and tools"</v>
       </c>
       <c r="R20" t="str">
@@ -2394,23 +2403,23 @@
         <v>"image":"https://i.postimg.cc/KYRDXVqg/ITESM.png"</v>
       </c>
       <c r="M21" t="str">
-        <f>CONCATENATE(C$1,$M$1,C21)</f>
+        <f t="shared" si="6"/>
         <v>"category":"Education"</v>
       </c>
       <c r="N21" t="str">
-        <f>CONCATENATE(D$1,$M$1,D21)</f>
+        <f t="shared" si="6"/>
         <v>"name":"Lean Enterprise"</v>
       </c>
       <c r="O21" t="str">
-        <f>CONCATENATE(E$1,$M$1,E21)</f>
+        <f t="shared" si="6"/>
         <v>"location":"CDMX"</v>
       </c>
       <c r="P21" t="str">
-        <f>CONCATENATE(F$1,$M$1,F21)</f>
+        <f t="shared" si="6"/>
         <v>"businessName":"ITESM"</v>
       </c>
       <c r="Q21" t="str">
-        <f>CONCATENATE(G$1,$M$1,G21)</f>
+        <f t="shared" si="6"/>
         <v>"description":"house of quality, pull, value mapping"</v>
       </c>
       <c r="R21" t="str">
@@ -2463,23 +2472,23 @@
         <v>"image":"https://i.postimg.cc/cLDBbZmS/MITX.png"</v>
       </c>
       <c r="M22" t="str">
-        <f>CONCATENATE(C$1,$M$1,C22)</f>
+        <f t="shared" si="6"/>
         <v>"category":"Education"</v>
       </c>
       <c r="N22" t="str">
-        <f>CONCATENATE(D$1,$M$1,D22)</f>
+        <f t="shared" si="6"/>
         <v>"name":"Supply chain fundamentals"</v>
       </c>
       <c r="O22" t="str">
-        <f>CONCATENATE(E$1,$M$1,E22)</f>
+        <f t="shared" si="6"/>
         <v>"location":"online"</v>
       </c>
       <c r="P22" t="str">
-        <f>CONCATENATE(F$1,$M$1,F22)</f>
+        <f t="shared" si="6"/>
         <v>"businessName":"MITx"</v>
       </c>
       <c r="Q22" t="str">
-        <f>CONCATENATE(G$1,$M$1,G22)</f>
+        <f t="shared" si="6"/>
         <v>"description":"Excel tools from demand planning to CSL and sales evaluations"</v>
       </c>
       <c r="R22" t="str">
@@ -2532,23 +2541,23 @@
         <v>"image":"https://i.postimg.cc/QMt08VtC/ADELAIDE.png"</v>
       </c>
       <c r="M23" t="str">
-        <f>CONCATENATE(C$1,$M$1,C23)</f>
+        <f t="shared" si="6"/>
         <v>"category":"Education"</v>
       </c>
       <c r="N23" t="str">
-        <f>CONCATENATE(D$1,$M$1,D23)</f>
+        <f t="shared" si="6"/>
         <v>"name":"Project Management"</v>
       </c>
       <c r="O23" t="str">
-        <f>CONCATENATE(E$1,$M$1,E23)</f>
+        <f t="shared" si="6"/>
         <v>"location":"online"</v>
       </c>
       <c r="P23" t="str">
-        <f>CONCATENATE(F$1,$M$1,F23)</f>
+        <f t="shared" si="6"/>
         <v>"businessName":"AldeideX"</v>
       </c>
       <c r="Q23" t="str">
-        <f>CONCATENATE(G$1,$M$1,G23)</f>
+        <f t="shared" si="6"/>
         <v>"description":"3 months basic course in project management BOK"</v>
       </c>
       <c r="R23" t="str">
@@ -2723,7 +2732,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
style adjusments in timeline
</commit_message>
<xml_diff>
--- a/src/recursos/BDD Timeline.xlsx
+++ b/src/recursos/BDD Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Files\Programming\portfolio\src\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D635B61E-6C20-4C68-8732-BE127092AB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765B00D7-2806-42AC-A882-BABC3BCE25E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
   </bookViews>
   <sheets>
     <sheet name="work exp" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="195">
   <si>
     <t>Name</t>
   </si>
@@ -550,15 +561,6 @@
     <t>"AldeideX"</t>
   </si>
   <si>
-    <t>"Virtual kitchen"</t>
-  </si>
-  <si>
-    <t>"Ecological Reserve"</t>
-  </si>
-  <si>
-    <t>"Restaurant / Bar"</t>
-  </si>
-  <si>
     <t>"Oil, Gas and Air filter manufacturing site"</t>
   </si>
   <si>
@@ -599,6 +601,30 @@
   </si>
   <si>
     <t>"language"</t>
+  </si>
+  <si>
+    <t>I was responsable of managing a fully virtual kitchen that prepares and delivers food this include overseeing kitchen operations, managing staff, maintaining food safety standards, overseeing delivery operations, and financial management, to archive this tasks i developed strong business skills, excellent communication skills and self-motivation.</t>
+  </si>
+  <si>
+    <t>As an Ecological Park Event Coordinator, I planned and executed eco-friendly events at a park, ensuring sustainability and conservation. Responsibilities included event planning, managing logistics, marketing, customer service, and promoting eco-friendly practices.</t>
+  </si>
+  <si>
+    <t>As a Restaurant Inventory Manager I was responsable for overseeing inventory levels of food and supplies for a restaurant, managing relationships with suppliers, monitoring costs, conducting audits, and reporting data to management.</t>
+  </si>
+  <si>
+    <t>As a Supply Chain Coordinator i was responsible for coordinating the movement of goods and materials from material suppliers and reviewing finished product inventory levels also, tracking purchese and manufacturing orders, coordinating with suppliers and logistics providers, and resolving any issues that arise in the supply chain. I develped organizational and communication skills, and learned detail-oriented perspective.</t>
+  </si>
+  <si>
+    <t>As a Demand Planner i was responsible for forecasting customer demand and developing production plans to meet that demand including analyzing market trends, developing sales forecasts, and collaborating with sales teams to ensure accurate demand planning i developed analytical and problem-solving skills</t>
+  </si>
+  <si>
+    <t>As a Planner Buyer i was  responsible for managing inventory levels and purchasing materials to meet production requirements including analyzing inventory levels, forecasting demand, and collaborating with suppliers to ensure timely delivery and testing of materials.</t>
+  </si>
+  <si>
+    <t>As an Operations Scheduler, i was responsible for developing and managing schedules for operational activities, such as production, maintenance, laboratory and regulatory it consisted of analyzing capacity constraints, coordinating with cross-functional teams, and communicating schedule changes to all deparments.</t>
+  </si>
+  <si>
+    <t>As a Industrial Engineer in a Pharmaceuticals Manufacturing and Packaging Plant, i was responsible for studing optimizing manufacturing processes to challenge standard manufacturing times it included analyzing production data, developing process improvements, and collaborating with cross-functional teams to ensure standard costs.</t>
   </si>
 </sst>
 </file>
@@ -652,7 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -660,6 +686,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -975,15 +1004,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08630837-D9DA-4E92-997A-E80AD53DE965}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:XFD43"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -1004,7 +1033,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>115</v>
@@ -1049,905 +1078,905 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="G2" t="s">
-        <v>173</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="K2" t="str">
+      <c r="K2" s="6" t="str">
         <f t="shared" ref="K2:K23" si="0">CONCATENATE(A$1,$M$1,A2)</f>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L2" t="str">
+      <c r="L2" s="6" t="str">
         <f>CONCATENATE(B$1,$M$1,$O$1,B2,$O$1)</f>
         <v>"image":"https://i.postimg.cc/BvVNXsLg/ARREL.png"</v>
       </c>
-      <c r="M2" t="str">
+      <c r="M2" s="6" t="str">
         <f t="shared" ref="M2:Q17" si="1">CONCATENATE(C$1,$M$1,C2)</f>
         <v>"category":"Work"</v>
       </c>
-      <c r="N2" t="str">
+      <c r="N2" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Owner"</v>
       </c>
-      <c r="O2" t="str">
+      <c r="O2" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"CDMX"</v>
       </c>
-      <c r="P2" t="str">
+      <c r="P2" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Arracheras Relamágo"</v>
       </c>
-      <c r="Q2" t="str">
-        <f t="shared" si="1"/>
-        <v>"description":"Virtual kitchen"</v>
-      </c>
-      <c r="R2" t="str">
+      <c r="Q2" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>"description":I was responsable of managing a fully virtual kitchen that prepares and delivers food this include overseeing kitchen operations, managing staff, maintaining food safety standards, overseeing delivery operations, and financial management, to archive this tasks i developed strong business skills, excellent communication skills and self-motivation.</v>
+      </c>
+      <c r="R2" s="6" t="str">
         <f>CONCATENATE(H$1,$M$1,$O$1,H2,$O$1)</f>
         <v>"begin":"01/03/2021"</v>
       </c>
-      <c r="S2" t="str">
+      <c r="S2" s="6" t="str">
         <f>CONCATENATE(I$1,$M$1,$O$1,I2,$O$1)</f>
         <v>"end":"01/04/2023"</v>
       </c>
-      <c r="U2" t="str">
+      <c r="U2" s="6" t="str">
         <f>CONCATENATE($K$1,K2,$N$1,L2,$N$1,M2,$N$1,N2,$N$1,O2,$N$1,P2,$N$1,Q2,$N$1,R2,$N$1,S2,$L$1)</f>
-        <v>{"language":"ENG","image":"https://i.postimg.cc/BvVNXsLg/ARREL.png","category":"Work","name":"Owner","location":"CDMX","businessName":"Arracheras Relamágo","description":"Virtual kitchen","begin":"01/03/2021","end":"01/04/2023"}</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="5" t="s">
+        <v>{"language":"ENG","image":"https://i.postimg.cc/BvVNXsLg/ARREL.png","category":"Work","name":"Owner","location":"CDMX","businessName":"Arracheras Relamágo","description":I was responsable of managing a fully virtual kitchen that prepares and delivers food this include overseeing kitchen operations, managing staff, maintaining food safety standards, overseeing delivery operations, and financial management, to archive this tasks i developed strong business skills, excellent communication skills and self-motivation.,"begin":"01/03/2021","end":"01/04/2023"}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="G3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="K3" t="str">
+      <c r="K3" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L3" t="str">
+      <c r="L3" s="6" t="str">
         <f t="shared" ref="L3:L23" si="2">CONCATENATE(B$1,$M$1,$O$1,B3,$O$1)</f>
         <v>"image":"https://i.postimg.cc/bNhgGmJK/GUANACASTLE.png"</v>
       </c>
-      <c r="M3" t="str">
+      <c r="M3" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Work"</v>
       </c>
-      <c r="N3" t="str">
+      <c r="N3" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Event Coordinator"</v>
       </c>
-      <c r="O3" t="str">
+      <c r="O3" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"Chiapas"</v>
       </c>
-      <c r="P3" t="str">
+      <c r="P3" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Parque Guanacastle"</v>
       </c>
-      <c r="Q3" t="str">
-        <f t="shared" si="1"/>
-        <v>"description":"Ecological Reserve"</v>
-      </c>
-      <c r="R3" t="str">
+      <c r="Q3" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>"description":As an Ecological Park Event Coordinator, I planned and executed eco-friendly events at a park, ensuring sustainability and conservation. Responsibilities included event planning, managing logistics, marketing, customer service, and promoting eco-friendly practices.</v>
+      </c>
+      <c r="R3" s="6" t="str">
         <f t="shared" ref="R3:R23" si="3">CONCATENATE(H$1,$M$1,$O$1,H3,$O$1)</f>
         <v>"begin":"01/09/2020"</v>
       </c>
-      <c r="S3" t="str">
+      <c r="S3" s="6" t="str">
         <f t="shared" ref="S3:S23" si="4">CONCATENATE(I$1,$M$1,$O$1,I3,$O$1)</f>
         <v>"end":"01/03/2021"</v>
       </c>
-      <c r="U3" t="str">
+      <c r="U3" s="6" t="str">
         <f t="shared" ref="U3:U23" si="5">CONCATENATE($K$1,K3,$N$1,L3,$N$1,M3,$N$1,N3,$N$1,O3,$N$1,P3,$N$1,Q3,$N$1,R3,$N$1,S3,$L$1)</f>
-        <v>{"language":"ENG","image":"https://i.postimg.cc/bNhgGmJK/GUANACASTLE.png","category":"Work","name":"Event Coordinator","location":"Chiapas","businessName":"Parque Guanacastle","description":"Ecological Reserve","begin":"01/09/2020","end":"01/03/2021"}</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="5" t="s">
+        <v>{"language":"ENG","image":"https://i.postimg.cc/bNhgGmJK/GUANACASTLE.png","category":"Work","name":"Event Coordinator","location":"Chiapas","businessName":"Parque Guanacastle","description":As an Ecological Park Event Coordinator, I planned and executed eco-friendly events at a park, ensuring sustainability and conservation. Responsibilities included event planning, managing logistics, marketing, customer service, and promoting eco-friendly practices.,"begin":"01/09/2020","end":"01/03/2021"}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="G4" t="s">
-        <v>175</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="J4" t="s">
-        <v>113</v>
-      </c>
-      <c r="K4" t="str">
+      <c r="K4" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L4" t="str">
+      <c r="L4" s="6" t="str">
         <f t="shared" si="2"/>
         <v>"image":"https://i.postimg.cc/x8KPxzsx/BOSTONS.png"</v>
       </c>
-      <c r="M4" t="str">
+      <c r="M4" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Work"</v>
       </c>
-      <c r="N4" t="str">
+      <c r="N4" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Inventory management"</v>
       </c>
-      <c r="O4" t="str">
+      <c r="O4" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"Chiapas"</v>
       </c>
-      <c r="P4" t="str">
+      <c r="P4" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Bostons"</v>
       </c>
-      <c r="Q4" t="str">
-        <f t="shared" si="1"/>
-        <v>"description":"Restaurant / Bar"</v>
-      </c>
-      <c r="R4" t="str">
+      <c r="Q4" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>"description":As a Restaurant Inventory Manager I was responsable for overseeing inventory levels of food and supplies for a restaurant, managing relationships with suppliers, monitoring costs, conducting audits, and reporting data to management.</v>
+      </c>
+      <c r="R4" s="6" t="str">
         <f t="shared" si="3"/>
         <v>"begin":"01/09/2020"</v>
       </c>
-      <c r="S4" t="str">
+      <c r="S4" s="6" t="str">
         <f t="shared" si="4"/>
         <v>"end":"01/03/2021"</v>
       </c>
-      <c r="U4" t="str">
+      <c r="U4" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>{"language":"ENG","image":"https://i.postimg.cc/x8KPxzsx/BOSTONS.png","category":"Work","name":"Inventory management","location":"Chiapas","businessName":"Bostons","description":"Restaurant / Bar","begin":"01/09/2020","end":"01/03/2021"}</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="5" t="s">
+        <v>{"language":"ENG","image":"https://i.postimg.cc/x8KPxzsx/BOSTONS.png","category":"Work","name":"Inventory management","location":"Chiapas","businessName":"Bostons","description":As a Restaurant Inventory Manager I was responsable for overseeing inventory levels of food and supplies for a restaurant, managing relationships with suppliers, monitoring costs, conducting audits, and reporting data to management.,"begin":"01/09/2020","end":"01/03/2021"}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G5" t="s">
-        <v>173</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="G5" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="K5" t="str">
+      <c r="J5" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="K5" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L5" t="str">
+      <c r="L5" s="6" t="str">
         <f t="shared" si="2"/>
         <v>"image":"https://i.postimg.cc/BvVNXsLg/ARREL.png"</v>
       </c>
-      <c r="M5" t="str">
+      <c r="M5" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Work"</v>
       </c>
-      <c r="N5" t="str">
+      <c r="N5" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Owner"</v>
       </c>
-      <c r="O5" t="str">
+      <c r="O5" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"CDMX"</v>
       </c>
-      <c r="P5" t="str">
+      <c r="P5" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Arracheras"</v>
       </c>
-      <c r="Q5" t="str">
-        <f t="shared" si="1"/>
-        <v>"description":"Virtual kitchen"</v>
-      </c>
-      <c r="R5" t="str">
+      <c r="Q5" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>"description":I was responsable of managing a fully virtual kitchen that prepares and delivers food this include overseeing kitchen operations, managing staff, maintaining food safety standards, overseeing delivery operations, and financial management, to archive this tasks i developed strong business skills, excellent communication skills and self-motivation.</v>
+      </c>
+      <c r="R5" s="6" t="str">
         <f t="shared" si="3"/>
         <v>"begin":"01/02/2019"</v>
       </c>
-      <c r="S5" t="str">
+      <c r="S5" s="6" t="str">
         <f t="shared" si="4"/>
         <v>"end":"01/09/2020"</v>
       </c>
-      <c r="U5" t="str">
+      <c r="U5" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>{"language":"ENG","image":"https://i.postimg.cc/BvVNXsLg/ARREL.png","category":"Work","name":"Owner","location":"CDMX","businessName":"Arracheras","description":"Virtual kitchen","begin":"01/02/2019","end":"01/09/2020"}</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="5" t="s">
+        <v>{"language":"ENG","image":"https://i.postimg.cc/BvVNXsLg/ARREL.png","category":"Work","name":"Owner","location":"CDMX","businessName":"Arracheras","description":I was responsable of managing a fully virtual kitchen that prepares and delivers food this include overseeing kitchen operations, managing staff, maintaining food safety standards, overseeing delivery operations, and financial management, to archive this tasks i developed strong business skills, excellent communication skills and self-motivation.,"begin":"01/02/2019","end":"01/09/2020"}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="G6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="K6" t="str">
+      <c r="K6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L6" t="str">
+      <c r="L6" s="6" t="str">
         <f t="shared" si="2"/>
         <v>"image":"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
       </c>
-      <c r="M6" t="str">
+      <c r="M6" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Work"</v>
       </c>
-      <c r="N6" t="str">
+      <c r="N6" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Supply coordinator"</v>
       </c>
-      <c r="O6" t="str">
+      <c r="O6" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"EDOMEX"</v>
       </c>
-      <c r="P6" t="str">
+      <c r="P6" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Federal"</v>
       </c>
-      <c r="Q6" t="str">
-        <f t="shared" si="1"/>
-        <v>"description":"Oil, Gas and Air filter manufacturing site"</v>
-      </c>
-      <c r="R6" t="str">
+      <c r="Q6" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>"description":As a Supply Chain Coordinator i was responsible for coordinating the movement of goods and materials from material suppliers and reviewing finished product inventory levels also, tracking purchese and manufacturing orders, coordinating with suppliers and logistics providers, and resolving any issues that arise in the supply chain. I develped organizational and communication skills, and learned detail-oriented perspective.</v>
+      </c>
+      <c r="R6" s="6" t="str">
         <f t="shared" si="3"/>
         <v>"begin":"01/07/2018"</v>
       </c>
-      <c r="S6" t="str">
+      <c r="S6" s="6" t="str">
         <f t="shared" si="4"/>
         <v>"end":"01/12/2018"</v>
       </c>
-      <c r="U6" t="str">
+      <c r="U6" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>{"language":"ENG","image":"https://i.postimg.cc/50QgzG8M/FEDERAL.png","category":"Work","name":"Supply coordinator","location":"EDOMEX","businessName":"Federal","description":"Oil, Gas and Air filter manufacturing site","begin":"01/07/2018","end":"01/12/2018"}</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="5" t="s">
+        <v>{"language":"ENG","image":"https://i.postimg.cc/50QgzG8M/FEDERAL.png","category":"Work","name":"Supply coordinator","location":"EDOMEX","businessName":"Federal","description":As a Supply Chain Coordinator i was responsible for coordinating the movement of goods and materials from material suppliers and reviewing finished product inventory levels also, tracking purchese and manufacturing orders, coordinating with suppliers and logistics providers, and resolving any issues that arise in the supply chain. I develped organizational and communication skills, and learned detail-oriented perspective.,"begin":"01/07/2018","end":"01/12/2018"}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="G7" t="s">
-        <v>176</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="K7" t="str">
+      <c r="K7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L7" t="str">
+      <c r="L7" s="6" t="str">
         <f t="shared" si="2"/>
         <v>"image":"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
       </c>
-      <c r="M7" t="str">
+      <c r="M7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Work"</v>
       </c>
-      <c r="N7" t="str">
+      <c r="N7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Demand planner"</v>
       </c>
-      <c r="O7" t="str">
+      <c r="O7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"EDOMEX"</v>
       </c>
-      <c r="P7" t="str">
+      <c r="P7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Federal"</v>
       </c>
-      <c r="Q7" t="str">
-        <f t="shared" si="1"/>
-        <v>"description":"Oil, Gas and Air filter manufacturing site"</v>
-      </c>
-      <c r="R7" t="str">
+      <c r="Q7" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>"description":As a Demand Planner i was responsible for forecasting customer demand and developing production plans to meet that demand including analyzing market trends, developing sales forecasts, and collaborating with sales teams to ensure accurate demand planning i developed analytical and problem-solving skills</v>
+      </c>
+      <c r="R7" s="6" t="str">
         <f t="shared" si="3"/>
         <v>"begin":"01/04/2018"</v>
       </c>
-      <c r="S7" t="str">
+      <c r="S7" s="6" t="str">
         <f t="shared" si="4"/>
         <v>"end":"01/12/2018"</v>
       </c>
-      <c r="U7" t="str">
+      <c r="U7" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>{"language":"ENG","image":"https://i.postimg.cc/50QgzG8M/FEDERAL.png","category":"Work","name":"Demand planner","location":"EDOMEX","businessName":"Federal","description":"Oil, Gas and Air filter manufacturing site","begin":"01/04/2018","end":"01/12/2018"}</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="5" t="s">
+        <v>{"language":"ENG","image":"https://i.postimg.cc/50QgzG8M/FEDERAL.png","category":"Work","name":"Demand planner","location":"EDOMEX","businessName":"Federal","description":As a Demand Planner i was responsible for forecasting customer demand and developing production plans to meet that demand including analyzing market trends, developing sales forecasts, and collaborating with sales teams to ensure accurate demand planning i developed analytical and problem-solving skills,"begin":"01/04/2018","end":"01/12/2018"}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="G8" t="s">
-        <v>176</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="G8" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="K8" t="str">
+      <c r="K8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L8" t="str">
+      <c r="L8" s="6" t="str">
         <f t="shared" si="2"/>
         <v>"image":"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
       </c>
-      <c r="M8" t="str">
+      <c r="M8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Work"</v>
       </c>
-      <c r="N8" t="str">
+      <c r="N8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Planner Buyer"</v>
       </c>
-      <c r="O8" t="str">
+      <c r="O8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"EDOMEX"</v>
       </c>
-      <c r="P8" t="str">
+      <c r="P8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Federal"</v>
       </c>
-      <c r="Q8" t="str">
-        <f t="shared" si="1"/>
-        <v>"description":"Oil, Gas and Air filter manufacturing site"</v>
-      </c>
-      <c r="R8" t="str">
+      <c r="Q8" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>"description":As a Planner Buyer i was  responsible for managing inventory levels and purchasing materials to meet production requirements including analyzing inventory levels, forecasting demand, and collaborating with suppliers to ensure timely delivery and testing of materials.</v>
+      </c>
+      <c r="R8" s="6" t="str">
         <f t="shared" si="3"/>
         <v>"begin":"01/04/2018"</v>
       </c>
-      <c r="S8" t="str">
+      <c r="S8" s="6" t="str">
         <f t="shared" si="4"/>
         <v>"end":"01/07/2018"</v>
       </c>
-      <c r="U8" t="str">
+      <c r="U8" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>{"language":"ENG","image":"https://i.postimg.cc/50QgzG8M/FEDERAL.png","category":"Work","name":"Planner Buyer","location":"EDOMEX","businessName":"Federal","description":"Oil, Gas and Air filter manufacturing site","begin":"01/04/2018","end":"01/07/2018"}</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="5" t="s">
+        <v>{"language":"ENG","image":"https://i.postimg.cc/50QgzG8M/FEDERAL.png","category":"Work","name":"Planner Buyer","location":"EDOMEX","businessName":"Federal","description":As a Planner Buyer i was  responsible for managing inventory levels and purchasing materials to meet production requirements including analyzing inventory levels, forecasting demand, and collaborating with suppliers to ensure timely delivery and testing of materials.,"begin":"01/04/2018","end":"01/07/2018"}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="G9" t="s">
-        <v>176</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="G9" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="K9" t="str">
+      <c r="K9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L9" t="str">
+      <c r="L9" s="6" t="str">
         <f t="shared" si="2"/>
         <v>"image":"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
       </c>
-      <c r="M9" t="str">
+      <c r="M9" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Work"</v>
       </c>
-      <c r="N9" t="str">
+      <c r="N9" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Procurement"</v>
       </c>
-      <c r="O9" t="str">
+      <c r="O9" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"EDOMEX"</v>
       </c>
-      <c r="P9" t="str">
+      <c r="P9" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Federal"</v>
       </c>
-      <c r="Q9" t="str">
+      <c r="Q9" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"description":"Oil, Gas and Air filter manufacturing site"</v>
       </c>
-      <c r="R9" t="str">
+      <c r="R9" s="6" t="str">
         <f t="shared" si="3"/>
         <v>"begin":"01/01/2018"</v>
       </c>
-      <c r="S9" t="str">
+      <c r="S9" s="6" t="str">
         <f t="shared" si="4"/>
         <v>"end":"01/04/2018"</v>
       </c>
-      <c r="U9" t="str">
+      <c r="U9" s="6" t="str">
         <f t="shared" si="5"/>
         <v>{"language":"ENG","image":"https://i.postimg.cc/50QgzG8M/FEDERAL.png","category":"Work","name":"Procurement","location":"EDOMEX","businessName":"Federal","description":"Oil, Gas and Air filter manufacturing site","begin":"01/01/2018","end":"01/04/2018"}</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="G10" t="s">
-        <v>177</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="G10" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="K10" t="str">
+      <c r="K10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L10" t="str">
+      <c r="L10" s="6" t="str">
         <f t="shared" si="2"/>
         <v>"image":"https://i.postimg.cc/Y9FN0Fwr/TEVA.png"</v>
       </c>
-      <c r="M10" t="str">
+      <c r="M10" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Work"</v>
       </c>
-      <c r="N10" t="str">
+      <c r="N10" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Operations Scheduler"</v>
       </c>
-      <c r="O10" t="str">
+      <c r="O10" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"CDMX"</v>
       </c>
-      <c r="P10" t="str">
+      <c r="P10" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Teva"</v>
       </c>
-      <c r="Q10" t="str">
-        <f t="shared" si="1"/>
-        <v>"description":"Oncological, OTC and inmunosuppresant manufactring and packaging site"</v>
-      </c>
-      <c r="R10" t="str">
+      <c r="Q10" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>"description":As an Operations Scheduler, i was responsible for developing and managing schedules for operational activities, such as production, maintenance, laboratory and regulatory it consisted of analyzing capacity constraints, coordinating with cross-functional teams, and communicating schedule changes to all deparments.</v>
+      </c>
+      <c r="R10" s="6" t="str">
         <f t="shared" si="3"/>
         <v>"begin":"01/06/2017"</v>
       </c>
-      <c r="S10" t="str">
+      <c r="S10" s="6" t="str">
         <f t="shared" si="4"/>
         <v>"end":"01/01/2018"</v>
       </c>
-      <c r="U10" t="str">
+      <c r="U10" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>{"language":"ENG","image":"https://i.postimg.cc/Y9FN0Fwr/TEVA.png","category":"Work","name":"Operations Scheduler","location":"CDMX","businessName":"Teva","description":"Oncological, OTC and inmunosuppresant manufactring and packaging site","begin":"01/06/2017","end":"01/01/2018"}</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="5" t="s">
+        <v>{"language":"ENG","image":"https://i.postimg.cc/Y9FN0Fwr/TEVA.png","category":"Work","name":"Operations Scheduler","location":"CDMX","businessName":"Teva","description":As an Operations Scheduler, i was responsible for developing and managing schedules for operational activities, such as production, maintenance, laboratory and regulatory it consisted of analyzing capacity constraints, coordinating with cross-functional teams, and communicating schedule changes to all deparments.,"begin":"01/06/2017","end":"01/01/2018"}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="G11" t="s">
-        <v>177</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="G11" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="K11" t="str">
+      <c r="K11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L11" t="str">
+      <c r="L11" s="6" t="str">
         <f t="shared" si="2"/>
         <v>"image":"https://i.postimg.cc/Y9FN0Fwr/TEVA.png"</v>
       </c>
-      <c r="M11" t="str">
+      <c r="M11" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Work"</v>
       </c>
-      <c r="N11" t="str">
+      <c r="N11" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Industrial Engineer"</v>
       </c>
-      <c r="O11" t="str">
+      <c r="O11" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"CDMX"</v>
       </c>
-      <c r="P11" t="str">
+      <c r="P11" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Teva"</v>
       </c>
-      <c r="Q11" t="str">
-        <f t="shared" si="1"/>
-        <v>"description":"Oncological, OTC and inmunosuppresant manufactring and packaging site"</v>
-      </c>
-      <c r="R11" t="str">
+      <c r="Q11" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>"description":As a Industrial Engineer in a Pharmaceuticals Manufacturing and Packaging Plant, i was responsible for studing optimizing manufacturing processes to challenge standard manufacturing times it included analyzing production data, developing process improvements, and collaborating with cross-functional teams to ensure standard costs.</v>
+      </c>
+      <c r="R11" s="6" t="str">
         <f t="shared" si="3"/>
         <v>"begin":"01/07/2014"</v>
       </c>
-      <c r="S11" t="str">
+      <c r="S11" s="6" t="str">
         <f t="shared" si="4"/>
         <v>"end":"01/06/2017"</v>
       </c>
-      <c r="U11" t="str">
+      <c r="U11" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>{"language":"ENG","image":"https://i.postimg.cc/Y9FN0Fwr/TEVA.png","category":"Work","name":"Industrial Engineer","location":"CDMX","businessName":"Teva","description":"Oncological, OTC and inmunosuppresant manufactring and packaging site","begin":"01/07/2014","end":"01/06/2017"}</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="5" t="s">
+        <v>{"language":"ENG","image":"https://i.postimg.cc/Y9FN0Fwr/TEVA.png","category":"Work","name":"Industrial Engineer","location":"CDMX","businessName":"Teva","description":As a Industrial Engineer in a Pharmaceuticals Manufacturing and Packaging Plant, i was responsible for studing optimizing manufacturing processes to challenge standard manufacturing times it included analyzing production data, developing process improvements, and collaborating with cross-functional teams to ensure standard costs.,"begin":"01/07/2014","end":"01/06/2017"}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="G12" t="s">
-        <v>177</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="G12" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="K12" t="str">
+      <c r="K12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L12" t="str">
+      <c r="L12" s="6" t="str">
         <f t="shared" si="2"/>
         <v>"image":"https://i.postimg.cc/Y9FN0Fwr/TEVA.png"</v>
       </c>
-      <c r="M12" t="str">
+      <c r="M12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Work"</v>
       </c>
-      <c r="N12" t="str">
+      <c r="N12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Jr process Engineer"</v>
       </c>
-      <c r="O12" t="str">
+      <c r="O12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"CDMX"</v>
       </c>
-      <c r="P12" t="str">
+      <c r="P12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Teva"</v>
       </c>
-      <c r="Q12" t="str">
+      <c r="Q12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"description":"Oncological, OTC and inmunosuppresant manufactring and packaging site"</v>
       </c>
-      <c r="R12" t="str">
+      <c r="R12" s="6" t="str">
         <f t="shared" si="3"/>
         <v>"begin":"01/10/2012"</v>
       </c>
-      <c r="S12" t="str">
+      <c r="S12" s="6" t="str">
         <f t="shared" si="4"/>
         <v>"end":"01/07/2014"</v>
       </c>
-      <c r="U12" t="str">
+      <c r="U12" s="6" t="str">
         <f t="shared" si="5"/>
         <v>{"language":"ENG","image":"https://i.postimg.cc/Y9FN0Fwr/TEVA.png","category":"Work","name":"Jr process Engineer","location":"CDMX","businessName":"Teva","description":"Oncological, OTC and inmunosuppresant manufactring and packaging site","begin":"01/10/2012","end":"01/07/2014"}</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="G13" t="s">
-        <v>178</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="G13" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="K13" t="str">
+      <c r="K13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L13" t="str">
+      <c r="L13" s="6" t="str">
         <f t="shared" si="2"/>
         <v>"image":"https://i.postimg.cc/x8Svzd0K/UNITEC.png"</v>
       </c>
-      <c r="M13" t="str">
+      <c r="M13" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Education"</v>
       </c>
-      <c r="N13" t="str">
+      <c r="N13" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Industrial Engineer"</v>
       </c>
-      <c r="O13" t="str">
+      <c r="O13" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"CDMX"</v>
       </c>
-      <c r="P13" t="str">
+      <c r="P13" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Unitec"</v>
       </c>
-      <c r="Q13" t="str">
+      <c r="Q13" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"description":"Bachelor's Degree"</v>
       </c>
-      <c r="R13" t="str">
+      <c r="R13" s="6" t="str">
         <f t="shared" si="3"/>
         <v>"begin":"01/09/2009"</v>
       </c>
-      <c r="S13" t="str">
+      <c r="S13" s="6" t="str">
         <f t="shared" si="4"/>
         <v>"end":"01/12/2012"</v>
       </c>
-      <c r="U13" t="str">
+      <c r="U13" s="6" t="str">
         <f t="shared" si="5"/>
         <v>{"language":"ENG","image":"https://i.postimg.cc/x8Svzd0K/UNITEC.png","category":"Education","name":"Industrial Engineer","location":"CDMX","businessName":"Unitec","description":"Bachelor's Degree","begin":"01/09/2009","end":"01/12/2012"}</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="G14" t="s">
-        <v>179</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="K14" t="str">
+      <c r="K14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>"language":"ENG"</v>
       </c>
-      <c r="L14" t="str">
+      <c r="L14" s="6" t="str">
         <f t="shared" si="2"/>
         <v>"image":"https://i.postimg.cc/VksFg5Xg/HENRY.png"</v>
       </c>
-      <c r="M14" t="str">
+      <c r="M14" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"category":"Education"</v>
       </c>
-      <c r="N14" t="str">
+      <c r="N14" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"name":"Full stack developer"</v>
       </c>
-      <c r="O14" t="str">
+      <c r="O14" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"location":"Argentina"</v>
       </c>
-      <c r="P14" t="str">
+      <c r="P14" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"businessName":"Henry"</v>
       </c>
-      <c r="Q14" t="str">
+      <c r="Q14" s="6" t="str">
         <f t="shared" si="1"/>
         <v>"description":"MERN + postgress &amp; redux certification"</v>
       </c>
-      <c r="R14" t="str">
+      <c r="R14" s="6" t="str">
         <f t="shared" si="3"/>
         <v>"begin":"01/02/2022"</v>
       </c>
-      <c r="S14" t="str">
+      <c r="S14" s="6" t="str">
         <f t="shared" si="4"/>
         <v>"end":"01/10/2022"</v>
       </c>
-      <c r="U14" t="str">
+      <c r="U14" s="6" t="str">
         <f t="shared" si="5"/>
         <v>{"language":"ENG","image":"https://i.postimg.cc/VksFg5Xg/HENRY.png","category":"Education","name":"Full stack developer","location":"Argentina","businessName":"Henry","description":"MERN + postgress &amp; redux certification","begin":"01/02/2022","end":"01/10/2022"}</v>
       </c>
@@ -1972,7 +2001,7 @@
         <v>168</v>
       </c>
       <c r="G15" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>92</v>
@@ -2041,7 +2070,7 @@
         <v>168</v>
       </c>
       <c r="G16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>87</v>
@@ -2110,7 +2139,7 @@
         <v>168</v>
       </c>
       <c r="G17" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>93</v>
@@ -2179,7 +2208,7 @@
         <v>169</v>
       </c>
       <c r="G18" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>94</v>
@@ -2248,7 +2277,7 @@
         <v>169</v>
       </c>
       <c r="G19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>94</v>
@@ -2317,7 +2346,7 @@
         <v>170</v>
       </c>
       <c r="G20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>95</v>
@@ -2386,7 +2415,7 @@
         <v>170</v>
       </c>
       <c r="G21" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>96</v>
@@ -2455,7 +2484,7 @@
         <v>171</v>
       </c>
       <c r="G22" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>97</v>
@@ -2524,7 +2553,7 @@
         <v>172</v>
       </c>
       <c r="G23" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>98</v>
@@ -2693,11 +2722,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J23" xr:uid="{08630837-D9DA-4E92-997A-E80AD53DE965}">
-    <filterColumn colId="9">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J23" xr:uid="{08630837-D9DA-4E92-997A-E80AD53DE965}"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{252060EC-65E3-493D-A711-C143D7CAFBEB}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{4EA91293-30D3-4D38-8DB9-AFDE2EDAD70C}"/>
@@ -2729,10 +2754,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACBE0D3-1FED-444E-85F3-AC56CB93C951}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3173,6 +3198,9 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="4"/>
     </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ended with timeline, added redux for articles, changing news to articles and make display for timeline cards
</commit_message>
<xml_diff>
--- a/src/recursos/BDD Timeline.xlsx
+++ b/src/recursos/BDD Timeline.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Files\Programming\portfolio\src\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA89251-0FEF-4D5E-8E91-0B92076B5B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5552A58C-7A1C-4DB7-889F-A35B33A95E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14025" yWindow="0" windowWidth="6465" windowHeight="10920" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10890" activeTab="1" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
   </bookViews>
   <sheets>
     <sheet name="work exp" sheetId="1" r:id="rId1"/>
     <sheet name="articles" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">articles!$A$1:$O$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'work exp'!$A$1:$J$23</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -29,29 +30,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="195">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="300">
   <si>
     <t>Location</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Sub-Category</t>
-  </si>
-  <si>
     <t>Logo</t>
   </si>
   <si>
-    <t>Photo</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>{</t>
   </si>
   <si>
@@ -64,162 +50,18 @@
     <t>,</t>
   </si>
   <si>
-    <t>'https://i.postimg.cc/BvVNXsLg/ARREL.png'</t>
-  </si>
-  <si>
     <t>'CDMX'</t>
   </si>
   <si>
-    <t>'Arracheras Relamágo'</t>
-  </si>
-  <si>
-    <t>'https://i.postimg.cc/bNhgGmJK/GUANACASTLE.png'</t>
-  </si>
-  <si>
-    <t>'Chiapas'</t>
-  </si>
-  <si>
-    <t>'Bostons'</t>
-  </si>
-  <si>
-    <t>'https://i.postimg.cc/50QgzG8M/FEDERAL.png'</t>
-  </si>
-  <si>
-    <t>'EDOMEX'</t>
-  </si>
-  <si>
-    <t>'Federal'</t>
-  </si>
-  <si>
-    <t>'https://i.postimg.cc/Y9FN0Fwr/TEVA.png'</t>
-  </si>
-  <si>
-    <t>'Teva'</t>
-  </si>
-  <si>
-    <t>'https://i.postimg.cc/VksFg5Xg/HENRY.png'</t>
-  </si>
-  <si>
-    <t>'Argentina'</t>
-  </si>
-  <si>
-    <t>'Henry'</t>
-  </si>
-  <si>
     <t>'Projects'</t>
   </si>
   <si>
-    <t>'Study rooms'</t>
-  </si>
-  <si>
-    <t>'Team certification project for full stack developer certification'</t>
-  </si>
-  <si>
-    <t>'https://i.postimg.cc/Wz6M6P3x/ITCHIO.webp'</t>
-  </si>
-  <si>
-    <t>'final boss'</t>
-  </si>
-  <si>
-    <t>'Game Jam'</t>
-  </si>
-  <si>
-    <t>'Hobby project to teach programming to my nephiew'</t>
-  </si>
-  <si>
     <t>'https://i.postimg.cc/59vpNhxB/DBGA.png'</t>
   </si>
   <si>
-    <t>'portfolio'</t>
-  </si>
-  <si>
     <t>'Personal'</t>
   </si>
   <si>
-    <t>'Personal project to promote my profile'</t>
-  </si>
-  <si>
-    <t>'countries'</t>
-  </si>
-  <si>
-    <t>'Individual project for certification'</t>
-  </si>
-  <si>
-    <t>'race control'</t>
-  </si>
-  <si>
-    <t>'Guanacastle'</t>
-  </si>
-  <si>
-    <t>'Enduro race control system based in excel'</t>
-  </si>
-  <si>
-    <t>'csl dashboard'</t>
-  </si>
-  <si>
-    <t>'OOS and CSL measuring tool'</t>
-  </si>
-  <si>
-    <t>'forecast evaluation tool'</t>
-  </si>
-  <si>
-    <t>'Deamnd planning evaluation tool'</t>
-  </si>
-  <si>
-    <t>'unit cost evaluation'</t>
-  </si>
-  <si>
-    <t>'Cost database evaluation tool'</t>
-  </si>
-  <si>
-    <t>'scheduling tool'</t>
-  </si>
-  <si>
-    <t>'Manufacturing planning and control tool'</t>
-  </si>
-  <si>
-    <t>'inventory tool'</t>
-  </si>
-  <si>
-    <t>'Inventory cost analysis tool'</t>
-  </si>
-  <si>
-    <t>'RCCP'</t>
-  </si>
-  <si>
-    <t>'Manufacturing time simulation for diferent volumes'</t>
-  </si>
-  <si>
-    <t>'site rate simulator'</t>
-  </si>
-  <si>
-    <t>'Cost center calculation tool'</t>
-  </si>
-  <si>
-    <t>'Budget control tool'</t>
-  </si>
-  <si>
-    <t>'Expenses by deparment follow up tool evaluating different scenarios'</t>
-  </si>
-  <si>
-    <t>'Control Dashboard'</t>
-  </si>
-  <si>
-    <t>'Data analysis dashboard with sales, inventory and category information'</t>
-  </si>
-  <si>
-    <t>'Business control'</t>
-  </si>
-  <si>
-    <t>'Sales, inventory, forecast and expenses follow up'</t>
-  </si>
-  <si>
-    <t>'Business design'</t>
-  </si>
-  <si>
-    <t>'business design and calculations'</t>
-  </si>
-  <si>
     <t>'Weight control'</t>
   </si>
   <si>
@@ -343,9 +185,6 @@
     <t>current</t>
   </si>
   <si>
-    <t>Langage</t>
-  </si>
-  <si>
     <t>01/04/2023</t>
   </si>
   <si>
@@ -614,6 +453,483 @@
   </si>
   <si>
     <t>As a Industrial Engineer in a Pharmaceuticals Manufacturing and Packaging Plant, i was responsible for studing optimizing manufacturing processes to challenge standard manufacturing times it included analyzing production data, developing process improvements, and collaborating with cross-functional teams to ensure standard costs.</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Industrial Engineering</t>
+  </si>
+  <si>
+    <t>Federal Mogul</t>
+  </si>
+  <si>
+    <t>Teva Pharmaceuticals</t>
+  </si>
+  <si>
+    <t>unit cost evaluation</t>
+  </si>
+  <si>
+    <t>Data science</t>
+  </si>
+  <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>Study rooms</t>
+  </si>
+  <si>
+    <t>portfolio</t>
+  </si>
+  <si>
+    <t>race control</t>
+  </si>
+  <si>
+    <t>csl dashboard</t>
+  </si>
+  <si>
+    <t>forecast evaluation tool</t>
+  </si>
+  <si>
+    <t>scheduling tool</t>
+  </si>
+  <si>
+    <t>RCCP</t>
+  </si>
+  <si>
+    <t>Budget control tool</t>
+  </si>
+  <si>
+    <t>Business control</t>
+  </si>
+  <si>
+    <t>Business design</t>
+  </si>
+  <si>
+    <t>Bostons</t>
+  </si>
+  <si>
+    <t>Arracheras Relamágo</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Guanacastle</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>CDMX</t>
+  </si>
+  <si>
+    <t>Chiapas</t>
+  </si>
+  <si>
+    <t>EDOMEX</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/59vpNhxB/DBGA.png</t>
+  </si>
+  <si>
+    <t>Team certification project for full stack developer certification</t>
+  </si>
+  <si>
+    <t>Personal project to promote my profile</t>
+  </si>
+  <si>
+    <t>Enduro race control system based in excel</t>
+  </si>
+  <si>
+    <t>Short description</t>
+  </si>
+  <si>
+    <t>OOS and CSL measuring tool based in excel</t>
+  </si>
+  <si>
+    <t>Demand planning evaluation tool  based in sales history</t>
+  </si>
+  <si>
+    <t>Cost database evaluation tool fed through erp system</t>
+  </si>
+  <si>
+    <t>Manufacturing planning and control tool with erp and excel</t>
+  </si>
+  <si>
+    <t>Manufacturing time simulation for diferent sales volumes</t>
+  </si>
+  <si>
+    <t>Expenses by deparment follow up tool evaluating different scenarios with excel and oracle</t>
+  </si>
+  <si>
+    <t>Sales, inventory, forecast and expenses follow up in excel</t>
+  </si>
+  <si>
+    <t>Problem description</t>
+  </si>
+  <si>
+    <t>Must develop a certification project to show understanding of all the tools learned in the course</t>
+  </si>
+  <si>
+    <t>Must track individual results of an enduro race conducted in chiapas</t>
+  </si>
+  <si>
+    <t>Production results weren't satisfactory and there were costumer complaints for lacking products</t>
+  </si>
+  <si>
+    <t>Forecasting method was lost due to a firing, must develop a sales forecasting system</t>
+  </si>
+  <si>
+    <t>Irregular cost results for similar products sugest incorrect standard information on erp system</t>
+  </si>
+  <si>
+    <t>Multiple manufacturing levels and products result in difficult follow-up for manufacturing orders</t>
+  </si>
+  <si>
+    <t>improve controlling communication to manufacturing departments on budget and expense control</t>
+  </si>
+  <si>
+    <t>simplify business control and data visualization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">business design and start up </t>
+  </si>
+  <si>
+    <t>create perspective and organize tasks for business start up</t>
+  </si>
+  <si>
+    <t>Desired state</t>
+  </si>
+  <si>
+    <t>develop and deploy a web app within 1 month and comply with 10 tech objectives</t>
+  </si>
+  <si>
+    <t>Show through action development skills and process understanding to HR personel</t>
+  </si>
+  <si>
+    <t>record in a fast and accurate way race results for enduro race</t>
+  </si>
+  <si>
+    <t>ensure key products availability and easy understanding of current unavailable products issues</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Deliverable</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>Goals</t>
+  </si>
+  <si>
+    <t>comply with the following 10 objectives: Deployment, 3rd party auth, payment management, mixed filters, image hosting, web notifications, logical delete, local storage, reviews and ratings, admin dashboard.</t>
+  </si>
+  <si>
+    <t>Time Constraints</t>
+  </si>
+  <si>
+    <t>4 week project</t>
+  </si>
+  <si>
+    <t>stripe, axios, bcrypt, express, heroku, nodemailer, passport, sequelize, bootstrap, react, redux, sweetalert</t>
+  </si>
+  <si>
+    <t>have a tool where i can communicate my skills and experiences</t>
+  </si>
+  <si>
+    <t>create a public access tool to show off tools</t>
+  </si>
+  <si>
+    <t>asap (undefined)</t>
+  </si>
+  <si>
+    <t>firebase, express, axios, node, react, redux</t>
+  </si>
+  <si>
+    <t>have a list of competitors, with lap times and ranked places</t>
+  </si>
+  <si>
+    <t>1 week</t>
+  </si>
+  <si>
+    <t>barcode scanner, barcode tags, laptop</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>present a tool that displays in a simple and understandable way out of stock items and month's target deliverables, a cause analysis for lacking items and a fast description of item behaviour</t>
+  </si>
+  <si>
+    <t>2 weeks</t>
+  </si>
+  <si>
+    <t>1.- APCs (ERP), 2.- Excel</t>
+  </si>
+  <si>
+    <t>make an initial forecast and forecast evaluation tool for follow up and adjustments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deliver a usable sales forecasting system and a forecast accuracy, adjustment and continous improvement method </t>
+  </si>
+  <si>
+    <t>3 weeks</t>
+  </si>
+  <si>
+    <t>ensure standard costs for every finished product item</t>
+  </si>
+  <si>
+    <t>deliver a tool where all finished product items can be evaluated for differences and each item can be seen in detail for cost composition</t>
+  </si>
+  <si>
+    <t>1.- BPCs (ERP)</t>
+  </si>
+  <si>
+    <t>have a single source of truth easy to read for items in every manufacturing level for daily update and follow up with manufacturing departments</t>
+  </si>
+  <si>
+    <t>deliver an easy to use tool for schedule follow up</t>
+  </si>
+  <si>
+    <t>have a working business</t>
+  </si>
+  <si>
+    <t>design, execute, follow up and document the start up process for a business</t>
+  </si>
+  <si>
+    <t>6 months</t>
+  </si>
+  <si>
+    <t>1.- excel, 2.- internet</t>
+  </si>
+  <si>
+    <t>control standard operation</t>
+  </si>
+  <si>
+    <t>count with a toolset for business follow up</t>
+  </si>
+  <si>
+    <t>1 month</t>
+  </si>
+  <si>
+    <t>1.- excel</t>
+  </si>
+  <si>
+    <t>management will receive a weekly report with their expenses by category and department to control their expense and stay within budget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">improve the information available to management to take decisions on expenses </t>
+  </si>
+  <si>
+    <t>1.- oracle database 2.- excel</t>
+  </si>
+  <si>
+    <t>cost center rate calculation takes too much time and is often left as is from previous years</t>
+  </si>
+  <si>
+    <t>count with an easy, simple and reliable process for work center rate calculation and update</t>
+  </si>
+  <si>
+    <t>design a process for work center rate calculation based on year volume</t>
+  </si>
+  <si>
+    <t>1.-sales forecast, 2.- oracle expenses report, 3.- BPCS (erp), 4.- Excel</t>
+  </si>
+  <si>
+    <t>Rough cut capacity calculation</t>
+  </si>
+  <si>
+    <t>update a tool for capacity simulation with different volumes of production</t>
+  </si>
+  <si>
+    <t>management requested to update an excel tool for capacity calculation</t>
+  </si>
+  <si>
+    <t>deliver an updated excel that takes production volume, manufacturing time and calculates # of shifts and total plant ocupation</t>
+  </si>
+  <si>
+    <t>1.- Excel, 2.- ERP querys</t>
+  </si>
+  <si>
+    <t>Sales history</t>
+  </si>
+  <si>
+    <t>Developed a sales report to manage promotions and procurement savings impact</t>
+  </si>
+  <si>
+    <t>there is poor insight on sales data and ingredient priority for procurement savings negotiations with vendors</t>
+  </si>
+  <si>
+    <t>management must have a clear idea of sales data to make accurate promotion strategies and improve ingredients negotiation with vendors</t>
+  </si>
+  <si>
+    <t>deliver an easy to understand report of sales</t>
+  </si>
+  <si>
+    <t>1.- sales data query, 2.- excel</t>
+  </si>
+  <si>
+    <t>no man left behind</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/1z2cyH27/RAPAX.png</t>
+  </si>
+  <si>
+    <t>charity event to raise founds for a team mate with cancer</t>
+  </si>
+  <si>
+    <t>Anibal Medina from out Airsoft team was diagnosed with esophagus cancer, he has some expenses not covered by ensurance</t>
+  </si>
+  <si>
+    <t>get help from airsoft community to raise founds to support expenses from Anibal</t>
+  </si>
+  <si>
+    <t>get at least 30 persons to participate in out found raising event</t>
+  </si>
+  <si>
+    <t>(this website)</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/111t3yk0MyLf579RYi9HejuXT2_1SU2nT/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1SCU6l4I_HmHcrfM_EBNAUiJRcV--JBBL/edit?usp=share_link&amp;ouid=111106748391899127979&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1SG6Pmsw6BrGiipTxdP1N4YhRp79Bd-hW/edit?usp=share_link&amp;ouid=111106748391899127979&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/12WL_eXufuLUQeZ_sNKIVOZdHyu_Iy6wY/edit?usp=share_link&amp;ouid=111106748391899127979&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1q4Tjjp7FevVKemQG030K3535Fbczt_VJ/edit?usp=share_link&amp;ouid=111106748391899127979&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1bpEoxoXatVNBxlIrQ2bcMa4wnt3Y0cIN/edit?usp=share_link&amp;ouid=111106748391899127979&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/11i0mtn__y61NDD4BkZlY6OqNXzM2yH6h/edit?usp=share_link&amp;ouid=111106748391899127979&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1w8qV7G2ZAbNgz6QKBc5cqURjNKGmkp9Z/edit?usp=share_link&amp;ouid=111106748391899127979&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1nc89THeHdhfpHmEzkQp1dlZAfIPsI8Tc/edit?usp=share_link&amp;ouid=111106748391899127979&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1cf_RmIB5DHJ3gCzKumu8RF31jWkR2jOn/edit?usp=share_link&amp;ouid=111106748391899127979&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>https://study-rooms-gilt.vercel.app/</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1HyAh3-hmE101fsFLxvUrsMUm1HAH-UUj/edit?usp=share_link&amp;ouid=111106748391899127979&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1DRsO8mDteb_kG7xlSQKh9nwTp_IScGDp/edit?usp=share_link&amp;ouid=111106748391899127979&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/prgQXP5k/budget-contol.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/0y7njKfS/business-control.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/mrRwHZX5/control-de-vueltas.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/L5qBpJ5n/CSL.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/TP9cq8BY/Forecast.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/nV6wLxJ6/unit-cost.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/WpDHj3QG/scheduling-tool.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/zf0nHCRy/RCCP.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/W3ygXs8j/rate-calculator.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/V6vXqJjD/sales-history-tool.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/3r6FZFfp/kickoff.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/FRHVTWQb/no-man-left-behind.png</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/bJVHWxz7/hoshin.png</t>
+  </si>
+  <si>
+    <t>["Team voting on project theme name and content","Brainstorming 50 user stories","voting to reduce user stories to 13","match user stories with tech objectives","web visual design, priorities and responsabilities assigned","project development and daily follow up","Project deployment","Testing and bug squashing","Ffinnished project presentation."]</t>
+  </si>
+  <si>
+    <t>["design a virtual CV","add visual tools to improve experience","create a way to simplify publications for new projects and archivements","testing","take feedback from friends and family to improve functionalities", "publish"]</t>
+  </si>
+  <si>
+    <t>["Analize avaliable tools (bar code scanner, tags, excel template)","Test and adapt excel template to register lap number and time automaticly","Work excel template to make automatic ranking calculation ,best and worst times","Test and release","Use, and release results after the race"]</t>
+  </si>
+  <si>
+    <t>["Analize backlog and deliverable items","Check manufacturing orders and available materials","organize items in categories such as: available in inventory, wip, unscheduled and materials unavailable","Design and populate a dashboard for easy understanding and presentation."]</t>
+  </si>
+  <si>
+    <t>["Analize sales data from ERP","Categorize items by sales volume and variability","Take a forecasting method (winter holt model) and implement it to data up tu 2 months previous","Get forecast data for months -1 and -2 then make fitness test","Adjust to current month and present forecast to management","Evaluate, adjust and publish new forecast monthly"]</t>
+  </si>
+  <si>
+    <t>["Download item master, bom and routing information for every finnished product item","Make a display with cost integration for every single finnished product item","Make a list with all finnished product items, with lot size, production cost (routing) and materials cost (bom), check for variations on each  same family item","Check items with variations and request an update in documentation","Publish tools and make them available to costs department"]</t>
+  </si>
+  <si>
+    <t>["Download and analize data form ERP (transaction states, inventory, order status)","Load prodction plan","Match if there are closed orders for production plan items, then check for open orders, material inventory avaiblability, purchase order placed for materials","Match status for all finished products on all levels","Testing","Update and present on daily meeting checking with every deparment status of all materials and follow up on priorities and variations."]</t>
+  </si>
+  <si>
+    <t>["Download routing form ERP"," Ask planning for forecast","Update tool with current data and test with simulated data","Schedule meeting with manufacturing department to validate results","Send updated tool to management team"]</t>
+  </si>
+  <si>
+    <t>["Request next year sales forecast","Calculate year production volume","Calculate hour requirement by cost center","Take historic production expenses and cross it with historic volume to calculate actual production costs","Make a simulator for cost rates according to production volumes","Test application","Use tool to generate rates for each cost center","Get approval from management and ask IT to upload rates to ERP system."]</t>
+  </si>
+  <si>
+    <t>["Download expense detail from oracle data base","Organize information and check on unusual data","Group expenses by category and make a summary","Import different budget scenarios (monthly, quarterly, ytd) and compare against actual expense","Make a display and challenge data","Present tools to upper management","Share tool with department heads"]</t>
+  </si>
+  <si>
+    <t>["Download sales data","Create a pivot table to make a sales summary with different time scopes","Expand sales into ingredient requirements", "Testing","Send tool to management along with recomendations for savings negotiations"]</t>
+  </si>
+  <si>
+    <t>["Create item master, routing and bom database, create a log for expenses and sales, operations, evaluate and follow up on inventory","Create a blanace sheet by vendor and sales channel","Forecasting and sales trends","Evaluate item performance and calculate safety stocks for ingrredients","Test and add promotions and promotion performance","Present information with friends and family for continous improvement oportunities"]</t>
+  </si>
+  <si>
+    <t>["Design business logic for a virtual kitchen","Design menu","Process design","Quote materials","Integrate costs and budget","Purchase tools and equipment","Adapt spaces  for cooking","Test instalations"," Start production","Evaluate process accuracy"]</t>
+  </si>
+  <si>
+    <t>["Design cheap but entretaining airsoft activities","Ensure a location for the event","Make an invite","Send it to as many airsfoters as possible","Command and control the event","Deliver the founding to anibal","Send payment evidence to airsoft teams to ensure transparrency"]</t>
+  </si>
+  <si>
+    <t>Site rate simulator</t>
+  </si>
+  <si>
+    <t>Langauge</t>
   </si>
 </sst>
 </file>
@@ -623,7 +939,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,8 +955,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -650,6 +974,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -667,7 +997,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -678,12 +1008,116 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -995,9 +1429,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08630837-D9DA-4E92-997A-E80AD53DE965}">
   <dimension ref="A1:XFD43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,81 +1457,81 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>186</v>
+        <v>132</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>117</v>
+        <v>63</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>119</v>
+        <v>65</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="J1" t="s">
-        <v>112</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="N1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O1" t="s">
-        <v>114</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>121</v>
+        <v>67</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>187</v>
-      </c>
       <c r="H2" s="7" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
       <c r="K2" s="5" t="str">
         <f t="shared" ref="K2:K23" si="0">CONCATENATE(A$1,$M$1,A2)</f>
@@ -1142,31 +1576,31 @@
     </row>
     <row r="3" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>122</v>
+        <v>68</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>136</v>
+        <v>82</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>156</v>
+        <v>102</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>161</v>
+        <v>107</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>188</v>
+        <v>134</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="K3" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1211,31 +1645,31 @@
     </row>
     <row r="4" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>123</v>
+        <v>69</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>137</v>
+        <v>83</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>156</v>
+        <v>102</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>162</v>
+        <v>108</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="K4" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1280,34 +1714,34 @@
     </row>
     <row r="5" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>121</v>
+        <v>67</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>187</v>
-      </c>
       <c r="H5" s="7" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
       <c r="K5" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1352,31 +1786,31 @@
     </row>
     <row r="6" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>157</v>
+        <v>103</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>164</v>
+        <v>110</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>190</v>
+        <v>136</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="K6" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1421,31 +1855,31 @@
     </row>
     <row r="7" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>157</v>
+        <v>103</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>164</v>
+        <v>110</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>191</v>
+        <v>137</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="K7" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1490,31 +1924,31 @@
     </row>
     <row r="8" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>140</v>
+        <v>86</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>157</v>
+        <v>103</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>164</v>
+        <v>110</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>192</v>
+        <v>138</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="K8" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1559,31 +1993,31 @@
     </row>
     <row r="9" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>124</v>
+        <v>70</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>157</v>
+        <v>103</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>164</v>
+        <v>110</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>173</v>
+        <v>119</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="K9" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1628,31 +2062,31 @@
     </row>
     <row r="10" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>142</v>
+        <v>88</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>165</v>
+        <v>111</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>193</v>
+        <v>139</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="K10" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1697,31 +2131,31 @@
     </row>
     <row r="11" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>165</v>
+        <v>111</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>194</v>
+        <v>140</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="K11" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1766,31 +2200,31 @@
     </row>
     <row r="12" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>165</v>
+        <v>111</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>174</v>
+        <v>120</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="K12" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1835,31 +2269,31 @@
     </row>
     <row r="13" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>166</v>
+        <v>112</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>175</v>
+        <v>121</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="K13" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1904,31 +2338,31 @@
     </row>
     <row r="14" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>127</v>
+        <v>73</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>158</v>
+        <v>104</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>167</v>
+        <v>113</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>176</v>
+        <v>122</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="K14" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1973,31 +2407,31 @@
     </row>
     <row r="15" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>177</v>
+        <v>123</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="K15" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2042,31 +2476,31 @@
     </row>
     <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>147</v>
+        <v>93</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>178</v>
+        <v>124</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="K16" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2111,31 +2545,31 @@
     </row>
     <row r="17" spans="1:21 16384:16384" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="K17" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2180,31 +2614,31 @@
     </row>
     <row r="18" spans="1:21 16384:16384" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>149</v>
+        <v>95</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>157</v>
+        <v>103</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>169</v>
+        <v>115</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="K18" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2215,7 +2649,7 @@
         <v>"image":"https://i.postimg.cc/FHhT6TXj/APICS.png"</v>
       </c>
       <c r="M18" s="5" t="str">
-        <f t="shared" ref="M18:Q26" si="6">CONCATENATE(C$1,$M$1,C18)</f>
+        <f t="shared" ref="M18:Q23" si="6">CONCATENATE(C$1,$M$1,C18)</f>
         <v>"category":"Education"</v>
       </c>
       <c r="N18" s="5" t="str">
@@ -2249,31 +2683,31 @@
     </row>
     <row r="19" spans="1:21 16384:16384" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>150</v>
+        <v>96</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>157</v>
+        <v>103</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>169</v>
+        <v>115</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="K19" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2318,31 +2752,31 @@
     </row>
     <row r="20" spans="1:21 16384:16384" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>130</v>
+        <v>76</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>151</v>
+        <v>97</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>170</v>
+        <v>116</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>185</v>
+        <v>131</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="K20" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2387,31 +2821,31 @@
     </row>
     <row r="21" spans="1:21 16384:16384" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>130</v>
+        <v>76</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>152</v>
+        <v>98</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>170</v>
+        <v>116</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>182</v>
+        <v>128</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="K21" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2456,31 +2890,31 @@
     </row>
     <row r="22" spans="1:21 16384:16384" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>153</v>
+        <v>99</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>159</v>
+        <v>105</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>171</v>
+        <v>117</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>183</v>
+        <v>129</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>111</v>
+        <v>57</v>
       </c>
       <c r="K22" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2525,31 +2959,31 @@
     </row>
     <row r="23" spans="1:21 16384:16384" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="C23" s="5" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>154</v>
+        <v>100</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>159</v>
+        <v>105</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>172</v>
+        <v>118</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>184</v>
+        <v>130</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="K23" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2594,97 +3028,97 @@
     </row>
     <row r="24" spans="1:21 16384:16384" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="I24" s="8">
         <v>43917</v>
       </c>
       <c r="K24" s="5" t="str">
-        <f t="shared" ref="K24:K29" si="7">CONCATENATE(A$1,$M$1,A24)</f>
+        <f t="shared" ref="K24:K27" si="7">CONCATENATE(A$1,$M$1,A24)</f>
         <v>"language":"ENG"</v>
       </c>
       <c r="L24" s="5" t="str">
-        <f t="shared" ref="L24:L29" si="8">CONCATENATE(B$1,$M$1,$O$1,B24,$O$1)</f>
+        <f t="shared" ref="L24:L27" si="8">CONCATENATE(B$1,$M$1,$O$1,B24,$O$1)</f>
         <v>"image":"'https://i.postimg.cc/59vpNhxB/DBGA.png'"</v>
       </c>
       <c r="M24" s="5" t="str">
-        <f t="shared" ref="M24:M29" si="9">CONCATENATE(C$1,$M$1,C24)</f>
+        <f t="shared" ref="M24:M27" si="9">CONCATENATE(C$1,$M$1,C24)</f>
         <v>"category":'Projects'</v>
       </c>
       <c r="N24" s="5" t="str">
-        <f t="shared" ref="N24:N29" si="10">CONCATENATE(D$1,$M$1,D24)</f>
+        <f t="shared" ref="N24:N27" si="10">CONCATENATE(D$1,$M$1,D24)</f>
         <v>"name":'Weight control'</v>
       </c>
       <c r="O24" s="5" t="str">
-        <f t="shared" ref="O24:O29" si="11">CONCATENATE(E$1,$M$1,E24)</f>
+        <f t="shared" ref="O24:O27" si="11">CONCATENATE(E$1,$M$1,E24)</f>
         <v>"location":'CDMX'</v>
       </c>
       <c r="P24" s="5" t="str">
-        <f t="shared" ref="P24:P29" si="12">CONCATENATE(F$1,$M$1,F24)</f>
+        <f t="shared" ref="P24:P27" si="12">CONCATENATE(F$1,$M$1,F24)</f>
         <v>"businessName":'Personal'</v>
       </c>
       <c r="Q24" s="5" t="str">
-        <f t="shared" ref="Q24:Q29" si="13">CONCATENATE(G$1,$M$1,G24)</f>
+        <f t="shared" ref="Q24:Q27" si="13">CONCATENATE(G$1,$M$1,G24)</f>
         <v>"description":'lost 20 kg in 2 years'</v>
       </c>
       <c r="R24" s="5" t="str">
-        <f t="shared" ref="R24:R29" si="14">CONCATENATE(H$1,$M$1,$O$1,H24,$O$1)</f>
+        <f t="shared" ref="R24:R27" si="14">CONCATENATE(H$1,$M$1,$O$1,H24,$O$1)</f>
         <v>"begin":"13/02/2018"</v>
       </c>
       <c r="S24" s="5" t="str">
-        <f t="shared" ref="S24:S29" si="15">CONCATENATE(I$1,$M$1,$O$1,I24,$O$1)</f>
+        <f t="shared" ref="S24:S27" si="15">CONCATENATE(I$1,$M$1,$O$1,I24,$O$1)</f>
         <v>"end":"43917"</v>
       </c>
       <c r="U24" s="5" t="str">
-        <f t="shared" ref="U24:U29" si="16">CONCATENATE($K$1,K24,$N$1,L24,$N$1,M24,$N$1,N24,$N$1,O24,$N$1,P24,$N$1,Q24,$N$1,R24,$N$1,S24,$L$1)</f>
+        <f t="shared" ref="U24:U27" si="16">CONCATENATE($K$1,K24,$N$1,L24,$N$1,M24,$N$1,N24,$N$1,O24,$N$1,P24,$N$1,Q24,$N$1,R24,$N$1,S24,$L$1)</f>
         <v>{"language":"ENG","image":"'https://i.postimg.cc/59vpNhxB/DBGA.png'","category":'Projects',"name":'Weight control',"location":'CDMX',"businessName":'Personal',"description":'lost 20 kg in 2 years',"begin":"13/02/2018","end":"43917"}</v>
       </c>
     </row>
     <row r="25" spans="1:21 16384:16384" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="I25" s="8">
         <v>41104</v>
@@ -2732,28 +3166,28 @@
     </row>
     <row r="26" spans="1:21 16384:16384" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="I26" s="8">
         <v>44271</v>
@@ -2801,31 +3235,31 @@
     </row>
     <row r="27" spans="1:21 16384:16384" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="F27" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="G27" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="I27" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="K27" s="5" t="str">
         <f t="shared" si="7"/>
@@ -2898,96 +3332,20 @@
     <row r="32" spans="1:21 16384:16384" x14ac:dyDescent="0.25">
       <c r="XFD32" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H40" s="3"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" t="s">
-        <v>65</v>
-      </c>
-      <c r="C41" t="s">
-        <v>66</v>
-      </c>
-      <c r="D41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" t="s">
-        <v>12</v>
-      </c>
-      <c r="F41" t="s">
-        <v>67</v>
-      </c>
-      <c r="G41" t="s">
-        <v>68</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="I41" s="4">
-        <v>41104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" t="s">
-        <v>70</v>
-      </c>
-      <c r="E42" t="s">
-        <v>71</v>
-      </c>
-      <c r="F42" t="s">
-        <v>72</v>
-      </c>
-      <c r="G42" t="s">
-        <v>73</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I42" s="4">
-        <v>44271</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" t="s">
-        <v>66</v>
-      </c>
-      <c r="D43" t="s">
-        <v>75</v>
-      </c>
-      <c r="E43" t="s">
-        <v>71</v>
-      </c>
-      <c r="F43" t="s">
-        <v>76</v>
-      </c>
-      <c r="G43" t="s">
-        <v>77</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I43" t="s">
-        <v>103</v>
-      </c>
+    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H41" s="3"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H42" s="3"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H43" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3021,452 +3379,797 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACBE0D3-1FED-444E-85F3-AC56CB93C951}">
-  <dimension ref="A1:Q18"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A1:O15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="66" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="83" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="114.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="131" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="189.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="96.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="53" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="144" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G1" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="16"/>
+    </row>
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="4"/>
+    </row>
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="4"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
-      </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="4"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>42</v>
-      </c>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="4"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="4"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" t="s">
-        <v>46</v>
-      </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="4"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" t="s">
-        <v>48</v>
-      </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="4"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" t="s">
-        <v>50</v>
-      </c>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="4"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" t="s">
-        <v>52</v>
-      </c>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="4"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" t="s">
-        <v>54</v>
-      </c>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="4"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" t="s">
-        <v>56</v>
-      </c>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="4"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" t="s">
-        <v>58</v>
-      </c>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="4"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" t="s">
-        <v>60</v>
-      </c>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="4"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" t="s">
-        <v>62</v>
-      </c>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="4"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
+      <c r="E15" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O15" xr:uid="{DACBE0D3-1FED-444E-85F3-AC56CB93C951}">
+    <filterColumn colId="0">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O15">
+      <sortCondition sortBy="cellColor" ref="A1:A15" dxfId="2"/>
+    </sortState>
+  </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1" xr:uid="{D5AB55C9-B0E6-4294-820E-7264AD3AC4A9}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{DAD769E2-F919-46EA-9826-4A3A95094776}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{DA58FBD3-A531-4FAF-A660-13EBE65967A4}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{6DF98C11-E740-447A-BB1C-1A93B5A891DB}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{306275F2-92C1-4503-BA0F-EDB80324B731}"/>
+    <hyperlink ref="F11" r:id="rId6" xr:uid="{CF9FCE47-D5A2-4D69-8C40-D4C64D534A8E}"/>
+    <hyperlink ref="F12" r:id="rId7" xr:uid="{2814EC2F-CE70-402C-8950-006DBF4E5E08}"/>
+    <hyperlink ref="F13" r:id="rId8" xr:uid="{1A842832-3FC2-48FE-B683-F5382A216B71}"/>
+    <hyperlink ref="F14" r:id="rId9" xr:uid="{AB31D706-35AD-460F-8E40-8BB54B871C4D}"/>
+    <hyperlink ref="F5" r:id="rId10" xr:uid="{B17BD6B2-73AB-45C4-B814-0452D99EB8CB}"/>
+    <hyperlink ref="F4" r:id="rId11" xr:uid="{DD09F1A0-7FA8-4A7E-83BC-E492F58B83A1}"/>
+    <hyperlink ref="F3" r:id="rId12" xr:uid="{763EB581-3C7F-4536-9511-C436874F6D99}"/>
+    <hyperlink ref="F2" r:id="rId13" xr:uid="{72CAF257-10DA-4E0D-BB2E-DC56256F4B95}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{F8B839E1-8BE9-4F97-9DFB-B533A619B800}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed all problems with the main pages, solved problems with redux - react - link, added maintenance
</commit_message>
<xml_diff>
--- a/src/recursos/BDD Timeline.xlsx
+++ b/src/recursos/BDD Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Files\Programming\portfolio\src\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D758B580-2F54-4DAA-B274-CA58022E685B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD81854-BA1D-4BB6-B6DC-2A739437DCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
+    <workbookView xWindow="0" yWindow="2490" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
   </bookViews>
   <sheets>
     <sheet name="work exp" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="388">
   <si>
     <t>Location</t>
   </si>
@@ -1067,9 +1067,6 @@
     <t>40 hrs a week</t>
   </si>
   <si>
-    <t>skillls</t>
-  </si>
-  <si>
     <t>Role: Business Owner</t>
   </si>
   <si>
@@ -1134,6 +1131,69 @@
   </si>
   <si>
     <t>Business Description:Bostons is the only sports bar in Tuxtla Gutierrez, Chiapas that specializes in selling delicious pizzas and snacks. Our fun and welcoming atmosphere is perfect for sports enthusiasts and food lovers alike. We are committed to providing high-quality food and excellent customer service, ensuring that every customer leaves satisfied. At Bostons, we understand the importance of maintaining inventory levels to ensure that we can always meet customer demand. That's why we have a dedicated team of inventory managers who oversee our supply levels and work closely with our suppliers to optimize costs and keep our prices competitive.</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>BusinessName</t>
+  </si>
+  <si>
+    <t>BusinessDescription</t>
+  </si>
+  <si>
+    <t>JobDescription</t>
+  </si>
+  <si>
+    <t>WorkTime</t>
+  </si>
+  <si>
+    <t>Begin</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>&lt;label&gt;</t>
+  </si>
+  <si>
+    <t>:&lt;/label&gt;&lt;input name="</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> value={this.state.timeline.</t>
+  </si>
+  <si>
+    <t>} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>ShortDescription</t>
+  </si>
+  <si>
+    <t>ProblemDescription</t>
+  </si>
+  <si>
+    <t>DesiredState</t>
+  </si>
+  <si>
+    <t>TimeConstraints</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> value={this.state.article.</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1203,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1173,8 +1233,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1184,12 +1249,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1213,7 +1272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1223,41 +1282,23 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1567,10 +1608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08630837-D9DA-4E92-997A-E80AD53DE965}">
-  <dimension ref="A1:Z88"/>
+  <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView topLeftCell="I86" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88:I100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,7 +1637,6 @@
     <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -1619,7 +1659,7 @@
         <v>304</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>345</v>
+        <v>382</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>293</v>
@@ -1677,7 +1717,7 @@
       <c r="F2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="9"/>
       <c r="H2" s="4" t="s">
         <v>294</v>
       </c>
@@ -1709,23 +1749,23 @@
         <v>image:"https://i.postimg.cc/BvVNXsLg/ARREL.png"</v>
       </c>
       <c r="R2" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C2)</f>
+        <f t="shared" ref="R2:R23" si="1">CONCATENATE(C$1,$R$1,C2)</f>
         <v>category:"Work"</v>
       </c>
       <c r="S2" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D2)</f>
+        <f t="shared" ref="S2:S23" si="2">CONCATENATE(D$1,$R$1,D2)</f>
         <v>name:"Owner"</v>
       </c>
       <c r="T2" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E2)</f>
+        <f t="shared" ref="T2:T23" si="3">CONCATENATE(E$1,$R$1,E2)</f>
         <v>location:"CDMX"</v>
       </c>
       <c r="U2" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F2)</f>
+        <f t="shared" ref="U2:U23" si="4">CONCATENATE(F$1,$R$1,F2)</f>
         <v>businessName:"Arracheras Relamágo"</v>
       </c>
       <c r="V2" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I2)</f>
+        <f t="shared" ref="V2:V23" si="5">CONCATENATE(I$1,$R$1,I2)</f>
         <v>jobDescription:I was responsable of managing a fully virtual kitchen that prepares and delivers food this include overseeing kitchen operations, managing staff, maintaining food safety standards, overseeing delivery operations, and financial management, to archive this tasks i developed strong business skills, excellent communication skills and self-motivation.</v>
       </c>
       <c r="W2" s="4" t="str">
@@ -1761,7 +1801,7 @@
       <c r="F3" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G3" s="14"/>
+      <c r="G3" s="9"/>
       <c r="H3" s="4" t="s">
         <v>310</v>
       </c>
@@ -1787,40 +1827,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q3" s="4" t="str">
-        <f t="shared" ref="Q3:Q23" si="1">CONCATENATE(B$1,$R$1,$T$1,B3,$T$1)</f>
+        <f t="shared" ref="Q3:Q23" si="6">CONCATENATE(B$1,$R$1,$T$1,B3,$T$1)</f>
         <v>image:"https://i.postimg.cc/bNhgGmJK/GUANACASTLE.png"</v>
       </c>
       <c r="R3" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C3)</f>
+        <f t="shared" si="1"/>
         <v>category:"Work"</v>
       </c>
       <c r="S3" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D3)</f>
+        <f t="shared" si="2"/>
         <v>name:"Event Coordinator"</v>
       </c>
       <c r="T3" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E3)</f>
+        <f t="shared" si="3"/>
         <v>location:"Chiapas"</v>
       </c>
       <c r="U3" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F3)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Parque Guanacastle"</v>
       </c>
       <c r="V3" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I3)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:As an Ecological Park Event Coordinator, I planned and executed eco-friendly events at a park, ensuring sustainability and conservation. Responsibilities included event planning, managing logistics, marketing, customer service, and promoting eco-friendly practices.</v>
       </c>
       <c r="W3" s="4" t="str">
-        <f t="shared" ref="W3:W23" si="2">CONCATENATE(L$1,$R$1,$T$1,L3,$T$1)</f>
+        <f t="shared" ref="W3:W23" si="7">CONCATENATE(L$1,$R$1,$T$1,L3,$T$1)</f>
         <v>"begin":"01/09/2020"</v>
       </c>
       <c r="X3" s="4" t="str">
-        <f t="shared" ref="X3:X23" si="3">CONCATENATE(M$1,$R$1,$T$1,M3,$T$1)</f>
+        <f t="shared" ref="X3:X23" si="8">CONCATENATE(M$1,$R$1,$T$1,M3,$T$1)</f>
         <v>"end":"01/03/2021"</v>
       </c>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4" t="str">
-        <f t="shared" ref="Z3:Z23" si="4">CONCATENATE($P$1,P3,$S$1,Q3,$S$1,R3,$S$1,S3,$S$1,T3,$S$1,U3,$S$1,V3,$S$1,W3,$S$1,X3,$Q$1)</f>
+        <f t="shared" ref="Z3:Z23" si="9">CONCATENATE($P$1,P3,$S$1,Q3,$S$1,R3,$S$1,S3,$S$1,T3,$S$1,U3,$S$1,V3,$S$1,W3,$S$1,X3,$Q$1)</f>
         <v>{language:"ENG",image:"https://i.postimg.cc/bNhgGmJK/GUANACASTLE.png",category:"Work",name:"Event Coordinator",location:"Chiapas",businessName:"Parque Guanacastle",jobDescription:As an Ecological Park Event Coordinator, I planned and executed eco-friendly events at a park, ensuring sustainability and conservation. Responsibilities included event planning, managing logistics, marketing, customer service, and promoting eco-friendly practices.,"begin":"01/09/2020","end":"01/03/2021"}</v>
       </c>
     </row>
@@ -1869,40 +1909,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q4" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/x8KPxzsx/BOSTONS.png"</v>
+      </c>
+      <c r="R4" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/x8KPxzsx/BOSTONS.png"</v>
-      </c>
-      <c r="R4" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C4)</f>
         <v>category:"Work"</v>
       </c>
       <c r="S4" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D4)</f>
+        <f t="shared" si="2"/>
         <v>name:"Inventory management"</v>
       </c>
       <c r="T4" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E4)</f>
+        <f t="shared" si="3"/>
         <v>location:"Chiapas"</v>
       </c>
       <c r="U4" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F4)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Bostons"</v>
       </c>
       <c r="V4" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I4)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:As a Restaurant Inventory Manager I was responsable for overseeing inventory levels of food and supplies for a restaurant, managing relationships with suppliers, monitoring costs, conducting audits, and reporting data to management.</v>
       </c>
       <c r="W4" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/09/2020"</v>
       </c>
       <c r="X4" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/03/2021"</v>
       </c>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/x8KPxzsx/BOSTONS.png",category:"Work",name:"Inventory management",location:"Chiapas",businessName:"Bostons",jobDescription:As a Restaurant Inventory Manager I was responsable for overseeing inventory levels of food and supplies for a restaurant, managing relationships with suppliers, monitoring costs, conducting audits, and reporting data to management.,"begin":"01/09/2020","end":"01/03/2021"}</v>
       </c>
     </row>
@@ -1953,40 +1993,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q5" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/BvVNXsLg/ARREL.png"</v>
+      </c>
+      <c r="R5" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/BvVNXsLg/ARREL.png"</v>
-      </c>
-      <c r="R5" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C5)</f>
         <v>category:"Work"</v>
       </c>
       <c r="S5" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D5)</f>
+        <f t="shared" si="2"/>
         <v>name:"Owner"</v>
       </c>
       <c r="T5" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E5)</f>
+        <f t="shared" si="3"/>
         <v>location:"CDMX"</v>
       </c>
       <c r="U5" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F5)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Arracheras"</v>
       </c>
       <c r="V5" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I5)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:I was responsable of managing a fully virtual kitchen that prepares and delivers food this include overseeing kitchen operations, managing staff, maintaining food safety standards, overseeing delivery operations, and financial management, to archive this tasks i developed strong business skills, excellent communication skills and self-motivation.</v>
       </c>
       <c r="W5" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/02/2019"</v>
       </c>
       <c r="X5" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/09/2020"</v>
       </c>
       <c r="Y5" s="4"/>
       <c r="Z5" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/BvVNXsLg/ARREL.png",category:"Work",name:"Owner",location:"CDMX",businessName:"Arracheras",jobDescription:I was responsable of managing a fully virtual kitchen that prepares and delivers food this include overseeing kitchen operations, managing staff, maintaining food safety standards, overseeing delivery operations, and financial management, to archive this tasks i developed strong business skills, excellent communication skills and self-motivation.,"begin":"01/02/2019","end":"01/09/2020"}</v>
       </c>
     </row>
@@ -2035,40 +2075,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q6" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
+      </c>
+      <c r="R6" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
-      </c>
-      <c r="R6" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C6)</f>
         <v>category:"Work"</v>
       </c>
       <c r="S6" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D6)</f>
+        <f t="shared" si="2"/>
         <v>name:"Supply coordinator"</v>
       </c>
       <c r="T6" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E6)</f>
+        <f t="shared" si="3"/>
         <v>location:"EDOMEX"</v>
       </c>
       <c r="U6" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F6)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Federal"</v>
       </c>
       <c r="V6" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I6)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:As a Supply Chain Coordinator i was responsible for coordinating the movement of goods and materials from material suppliers and reviewing finished product inventory levels also, tracking purchese and manufacturing orders, coordinating with suppliers and logistics providers, and resolving any issues that arise in the supply chain. I develped organizational and communication skills, and learned detail-oriented perspective.</v>
       </c>
       <c r="W6" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/07/2018"</v>
       </c>
       <c r="X6" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/12/2018"</v>
       </c>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png",category:"Work",name:"Supply coordinator",location:"EDOMEX",businessName:"Federal",jobDescription:As a Supply Chain Coordinator i was responsible for coordinating the movement of goods and materials from material suppliers and reviewing finished product inventory levels also, tracking purchese and manufacturing orders, coordinating with suppliers and logistics providers, and resolving any issues that arise in the supply chain. I develped organizational and communication skills, and learned detail-oriented perspective.,"begin":"01/07/2018","end":"01/12/2018"}</v>
       </c>
     </row>
@@ -2117,40 +2157,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q7" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
+      </c>
+      <c r="R7" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
-      </c>
-      <c r="R7" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C7)</f>
         <v>category:"Work"</v>
       </c>
       <c r="S7" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D7)</f>
+        <f t="shared" si="2"/>
         <v>name:"Demand planner"</v>
       </c>
       <c r="T7" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E7)</f>
+        <f t="shared" si="3"/>
         <v>location:"EDOMEX"</v>
       </c>
       <c r="U7" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F7)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Federal"</v>
       </c>
       <c r="V7" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I7)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:As a Demand Planner i was responsible for forecasting customer demand and developing production plans to meet that demand including analyzing market trends, developing sales forecasts, and collaborating with sales teams to ensure accurate demand planning i developed analytical and problem-solving skills</v>
       </c>
       <c r="W7" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/04/2018"</v>
       </c>
       <c r="X7" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/12/2018"</v>
       </c>
       <c r="Y7" s="4"/>
       <c r="Z7" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png",category:"Work",name:"Demand planner",location:"EDOMEX",businessName:"Federal",jobDescription:As a Demand Planner i was responsible for forecasting customer demand and developing production plans to meet that demand including analyzing market trends, developing sales forecasts, and collaborating with sales teams to ensure accurate demand planning i developed analytical and problem-solving skills,"begin":"01/04/2018","end":"01/12/2018"}</v>
       </c>
     </row>
@@ -2199,40 +2239,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q8" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
+      </c>
+      <c r="R8" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
-      </c>
-      <c r="R8" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C8)</f>
         <v>category:"Work"</v>
       </c>
       <c r="S8" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D8)</f>
+        <f t="shared" si="2"/>
         <v>name:"Planner Buyer"</v>
       </c>
       <c r="T8" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E8)</f>
+        <f t="shared" si="3"/>
         <v>location:"EDOMEX"</v>
       </c>
       <c r="U8" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F8)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Federal"</v>
       </c>
       <c r="V8" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I8)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:As a Planner Buyer i was  responsible for managing inventory levels and purchasing materials to meet production requirements including analyzing inventory levels, forecasting demand, and collaborating with suppliers to ensure timely delivery and testing of materials.</v>
       </c>
       <c r="W8" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/04/2018"</v>
       </c>
       <c r="X8" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/07/2018"</v>
       </c>
       <c r="Y8" s="4"/>
       <c r="Z8" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png",category:"Work",name:"Planner Buyer",location:"EDOMEX",businessName:"Federal",jobDescription:As a Planner Buyer i was  responsible for managing inventory levels and purchasing materials to meet production requirements including analyzing inventory levels, forecasting demand, and collaborating with suppliers to ensure timely delivery and testing of materials.,"begin":"01/04/2018","end":"01/07/2018"}</v>
       </c>
     </row>
@@ -2281,40 +2321,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q9" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
+      </c>
+      <c r="R9" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png"</v>
-      </c>
-      <c r="R9" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C9)</f>
         <v>category:"Work"</v>
       </c>
       <c r="S9" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D9)</f>
+        <f t="shared" si="2"/>
         <v>name:"Procurement"</v>
       </c>
       <c r="T9" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E9)</f>
+        <f t="shared" si="3"/>
         <v>location:"EDOMEX"</v>
       </c>
       <c r="U9" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F9)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Federal"</v>
       </c>
       <c r="V9" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I9)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"Oil, Gas and Air filter manufacturing site"</v>
       </c>
       <c r="W9" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/01/2018"</v>
       </c>
       <c r="X9" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/04/2018"</v>
       </c>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/50QgzG8M/FEDERAL.png",category:"Work",name:"Procurement",location:"EDOMEX",businessName:"Federal",jobDescription:"Oil, Gas and Air filter manufacturing site","begin":"01/01/2018","end":"01/04/2018"}</v>
       </c>
     </row>
@@ -2363,40 +2403,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q10" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/Y9FN0Fwr/TEVA.png"</v>
+      </c>
+      <c r="R10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/Y9FN0Fwr/TEVA.png"</v>
-      </c>
-      <c r="R10" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C10)</f>
         <v>category:"Work"</v>
       </c>
       <c r="S10" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D10)</f>
+        <f t="shared" si="2"/>
         <v>name:"Operations Scheduler"</v>
       </c>
       <c r="T10" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E10)</f>
+        <f t="shared" si="3"/>
         <v>location:"CDMX"</v>
       </c>
       <c r="U10" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F10)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Teva"</v>
       </c>
       <c r="V10" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I10)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:As an Operations Scheduler, i was responsible for developing and managing schedules for operational activities, such as production, maintenance, laboratory and regulatory it consisted of analyzing capacity constraints, coordinating with cross-functional teams, and communicating schedule changes to all deparments.</v>
       </c>
       <c r="W10" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/06/2017"</v>
       </c>
       <c r="X10" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/01/2018"</v>
       </c>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/Y9FN0Fwr/TEVA.png",category:"Work",name:"Operations Scheduler",location:"CDMX",businessName:"Teva",jobDescription:As an Operations Scheduler, i was responsible for developing and managing schedules for operational activities, such as production, maintenance, laboratory and regulatory it consisted of analyzing capacity constraints, coordinating with cross-functional teams, and communicating schedule changes to all deparments.,"begin":"01/06/2017","end":"01/01/2018"}</v>
       </c>
     </row>
@@ -2445,40 +2485,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q11" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/Y9FN0Fwr/TEVA.png"</v>
+      </c>
+      <c r="R11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/Y9FN0Fwr/TEVA.png"</v>
-      </c>
-      <c r="R11" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C11)</f>
         <v>category:"Work"</v>
       </c>
       <c r="S11" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D11)</f>
+        <f t="shared" si="2"/>
         <v>name:"Industrial Engineer"</v>
       </c>
       <c r="T11" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E11)</f>
+        <f t="shared" si="3"/>
         <v>location:"CDMX"</v>
       </c>
       <c r="U11" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F11)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Teva"</v>
       </c>
       <c r="V11" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I11)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:As a Industrial Engineer in a Pharmaceuticals Manufacturing and Packaging Plant, i was responsible for studing optimizing manufacturing processes to challenge standard manufacturing times it included analyzing production data, developing process improvements, and collaborating with cross-functional teams to ensure standard costs.</v>
       </c>
       <c r="W11" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/07/2014"</v>
       </c>
       <c r="X11" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/06/2017"</v>
       </c>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/Y9FN0Fwr/TEVA.png",category:"Work",name:"Industrial Engineer",location:"CDMX",businessName:"Teva",jobDescription:As a Industrial Engineer in a Pharmaceuticals Manufacturing and Packaging Plant, i was responsible for studing optimizing manufacturing processes to challenge standard manufacturing times it included analyzing production data, developing process improvements, and collaborating with cross-functional teams to ensure standard costs.,"begin":"01/07/2014","end":"01/06/2017"}</v>
       </c>
     </row>
@@ -2527,40 +2567,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q12" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/Y9FN0Fwr/TEVA.png"</v>
+      </c>
+      <c r="R12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/Y9FN0Fwr/TEVA.png"</v>
-      </c>
-      <c r="R12" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C12)</f>
         <v>category:"Work"</v>
       </c>
       <c r="S12" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D12)</f>
+        <f t="shared" si="2"/>
         <v>name:"Jr process Engineer"</v>
       </c>
       <c r="T12" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E12)</f>
+        <f t="shared" si="3"/>
         <v>location:"CDMX"</v>
       </c>
       <c r="U12" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F12)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Teva"</v>
       </c>
       <c r="V12" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I12)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"Oncological, OTC and inmunosuppresant manufactring and packaging site"</v>
       </c>
       <c r="W12" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/10/2012"</v>
       </c>
       <c r="X12" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/07/2014"</v>
       </c>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/Y9FN0Fwr/TEVA.png",category:"Work",name:"Jr process Engineer",location:"CDMX",businessName:"Teva",jobDescription:"Oncological, OTC and inmunosuppresant manufactring and packaging site","begin":"01/10/2012","end":"01/07/2014"}</v>
       </c>
     </row>
@@ -2609,40 +2649,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q13" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/x8Svzd0K/UNITEC.png"</v>
+      </c>
+      <c r="R13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/x8Svzd0K/UNITEC.png"</v>
-      </c>
-      <c r="R13" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C13)</f>
         <v>category:"Education"</v>
       </c>
       <c r="S13" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D13)</f>
+        <f t="shared" si="2"/>
         <v>name:"Industrial Engineer"</v>
       </c>
       <c r="T13" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E13)</f>
+        <f t="shared" si="3"/>
         <v>location:"CDMX"</v>
       </c>
       <c r="U13" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F13)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Unitec"</v>
       </c>
       <c r="V13" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I13)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"Bachelor's Degree"</v>
       </c>
       <c r="W13" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/09/2009"</v>
       </c>
       <c r="X13" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/12/2012"</v>
       </c>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/x8Svzd0K/UNITEC.png",category:"Education",name:"Industrial Engineer",location:"CDMX",businessName:"Unitec",jobDescription:"Bachelor's Degree","begin":"01/09/2009","end":"01/12/2012"}</v>
       </c>
     </row>
@@ -2691,40 +2731,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q14" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/VksFg5Xg/HENRY.png"</v>
+      </c>
+      <c r="R14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/VksFg5Xg/HENRY.png"</v>
-      </c>
-      <c r="R14" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C14)</f>
         <v>category:"Education"</v>
       </c>
       <c r="S14" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D14)</f>
+        <f t="shared" si="2"/>
         <v>name:"Full stack developer"</v>
       </c>
       <c r="T14" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E14)</f>
+        <f t="shared" si="3"/>
         <v>location:"Argentina"</v>
       </c>
       <c r="U14" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F14)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"Henry"</v>
       </c>
       <c r="V14" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I14)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"MERN + postgress &amp; redux certification"</v>
       </c>
       <c r="W14" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/02/2022"</v>
       </c>
       <c r="X14" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/10/2022"</v>
       </c>
       <c r="Y14" s="4"/>
       <c r="Z14" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/VksFg5Xg/HENRY.png",category:"Education",name:"Full stack developer",location:"Argentina",businessName:"Henry",jobDescription:"MERN + postgress &amp; redux certification","begin":"01/02/2022","end":"01/10/2022"}</v>
       </c>
     </row>
@@ -2773,40 +2813,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q15" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/QCLbJbqK/CENCAD.png"</v>
+      </c>
+      <c r="R15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/QCLbJbqK/CENCAD.png"</v>
-      </c>
-      <c r="R15" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C15)</f>
         <v>category:"Education"</v>
       </c>
       <c r="S15" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D15)</f>
+        <f t="shared" si="2"/>
         <v>name:"Close space rescue operations"</v>
       </c>
       <c r="T15" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E15)</f>
+        <f t="shared" si="3"/>
         <v>location:"CDMX"</v>
       </c>
       <c r="U15" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F15)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"CENCAD"</v>
       </c>
       <c r="V15" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I15)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"Zonning, Equipment set up, rescue operations control"</v>
       </c>
       <c r="W15" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/02/2017"</v>
       </c>
       <c r="X15" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/02/2017"</v>
       </c>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/QCLbJbqK/CENCAD.png",category:"Education",name:"Close space rescue operations",location:"CDMX",businessName:"CENCAD",jobDescription:"Zonning, Equipment set up, rescue operations control","begin":"01/02/2017","end":"01/02/2017"}</v>
       </c>
     </row>
@@ -2855,40 +2895,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q16" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/QCLbJbqK/CENCAD.png"</v>
+      </c>
+      <c r="R16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/QCLbJbqK/CENCAD.png"</v>
-      </c>
-      <c r="R16" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C16)</f>
         <v>category:"Education"</v>
       </c>
       <c r="S16" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D16)</f>
+        <f t="shared" si="2"/>
         <v>name:"First aid training"</v>
       </c>
       <c r="T16" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E16)</f>
+        <f t="shared" si="3"/>
         <v>location:"CDMX"</v>
       </c>
       <c r="U16" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F16)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"CENCAD"</v>
       </c>
       <c r="V16" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I16)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"first aid for burns, bleeding and broken bones"</v>
       </c>
       <c r="W16" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/06/2017"</v>
       </c>
       <c r="X16" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/06/2017"</v>
       </c>
       <c r="Y16" s="4"/>
       <c r="Z16" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/QCLbJbqK/CENCAD.png",category:"Education",name:"First aid training",location:"CDMX",businessName:"CENCAD",jobDescription:"first aid for burns, bleeding and broken bones","begin":"01/06/2017","end":"01/06/2017"}</v>
       </c>
     </row>
@@ -2937,40 +2977,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q17" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/QCLbJbqK/CENCAD.png"</v>
+      </c>
+      <c r="R17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/QCLbJbqK/CENCAD.png"</v>
-      </c>
-      <c r="R17" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C17)</f>
         <v>category:"Education"</v>
       </c>
       <c r="S17" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D17)</f>
+        <f t="shared" si="2"/>
         <v>name:"Fire brigade training"</v>
       </c>
       <c r="T17" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E17)</f>
+        <f t="shared" si="3"/>
         <v>location:"CDMX"</v>
       </c>
       <c r="U17" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F17)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"CENCAD"</v>
       </c>
       <c r="V17" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I17)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"Equipment, rescue operations, fire containment"</v>
       </c>
       <c r="W17" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/10/2017"</v>
       </c>
       <c r="X17" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/10/2017"</v>
       </c>
       <c r="Y17" s="4"/>
       <c r="Z17" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/QCLbJbqK/CENCAD.png",category:"Education",name:"Fire brigade training",location:"CDMX",businessName:"CENCAD",jobDescription:"Equipment, rescue operations, fire containment","begin":"01/10/2017","end":"01/10/2017"}</v>
       </c>
     </row>
@@ -3019,40 +3059,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q18" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/FHhT6TXj/APICS.png"</v>
+      </c>
+      <c r="R18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/FHhT6TXj/APICS.png"</v>
-      </c>
-      <c r="R18" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C18)</f>
         <v>category:"Education"</v>
       </c>
       <c r="S18" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D18)</f>
+        <f t="shared" si="2"/>
         <v>name:"Inventory control"</v>
       </c>
       <c r="T18" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E18)</f>
+        <f t="shared" si="3"/>
         <v>location:"EDOMEX"</v>
       </c>
       <c r="U18" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F18)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"APICs"</v>
       </c>
       <c r="V18" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I18)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"reorder point, costs, ABC classification"</v>
       </c>
       <c r="W18" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/10/2018"</v>
       </c>
       <c r="X18" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/10/2018"</v>
       </c>
       <c r="Y18" s="4"/>
       <c r="Z18" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/FHhT6TXj/APICS.png",category:"Education",name:"Inventory control",location:"EDOMEX",businessName:"APICs",jobDescription:"reorder point, costs, ABC classification","begin":"01/10/2018","end":"01/10/2018"}</v>
       </c>
     </row>
@@ -3101,40 +3141,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q19" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/FHhT6TXj/APICS.png"</v>
+      </c>
+      <c r="R19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/FHhT6TXj/APICS.png"</v>
-      </c>
-      <c r="R19" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C19)</f>
         <v>category:"Education"</v>
       </c>
       <c r="S19" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D19)</f>
+        <f t="shared" si="2"/>
         <v>name:"Procurement planning"</v>
       </c>
       <c r="T19" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E19)</f>
+        <f t="shared" si="3"/>
         <v>location:"EDOMEX"</v>
       </c>
       <c r="U19" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F19)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"APICs"</v>
       </c>
       <c r="V19" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I19)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"sourcing, supplier management, OOS, CSL"</v>
       </c>
       <c r="W19" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/10/2018"</v>
       </c>
       <c r="X19" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/10/2018"</v>
       </c>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/FHhT6TXj/APICS.png",category:"Education",name:"Procurement planning",location:"EDOMEX",businessName:"APICs",jobDescription:"sourcing, supplier management, OOS, CSL","begin":"01/10/2018","end":"01/10/2018"}</v>
       </c>
     </row>
@@ -3183,40 +3223,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q20" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/KYRDXVqg/ITESM.png"</v>
+      </c>
+      <c r="R20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/KYRDXVqg/ITESM.png"</v>
-      </c>
-      <c r="R20" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C20)</f>
         <v>category:"Education"</v>
       </c>
       <c r="S20" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D20)</f>
+        <f t="shared" si="2"/>
         <v>name:"Six Sigma"</v>
       </c>
       <c r="T20" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E20)</f>
+        <f t="shared" si="3"/>
         <v>location:"CDMX"</v>
       </c>
       <c r="U20" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F20)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"ITESM"</v>
       </c>
       <c r="V20" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I20)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"DMAIC methodology and tools"</v>
       </c>
       <c r="W20" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/02/2013"</v>
       </c>
       <c r="X20" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/06/2013"</v>
       </c>
       <c r="Y20" s="4"/>
       <c r="Z20" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/KYRDXVqg/ITESM.png",category:"Education",name:"Six Sigma",location:"CDMX",businessName:"ITESM",jobDescription:"DMAIC methodology and tools","begin":"01/02/2013","end":"01/06/2013"}</v>
       </c>
     </row>
@@ -3265,40 +3305,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q21" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/KYRDXVqg/ITESM.png"</v>
+      </c>
+      <c r="R21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/KYRDXVqg/ITESM.png"</v>
-      </c>
-      <c r="R21" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C21)</f>
         <v>category:"Education"</v>
       </c>
       <c r="S21" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D21)</f>
+        <f t="shared" si="2"/>
         <v>name:"Lean Enterprise"</v>
       </c>
       <c r="T21" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E21)</f>
+        <f t="shared" si="3"/>
         <v>location:"CDMX"</v>
       </c>
       <c r="U21" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F21)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"ITESM"</v>
       </c>
       <c r="V21" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I21)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"house of quality, pull, value mapping"</v>
       </c>
       <c r="W21" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/08/2014"</v>
       </c>
       <c r="X21" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/10/2014"</v>
       </c>
       <c r="Y21" s="4"/>
       <c r="Z21" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/KYRDXVqg/ITESM.png",category:"Education",name:"Lean Enterprise",location:"CDMX",businessName:"ITESM",jobDescription:"house of quality, pull, value mapping","begin":"01/08/2014","end":"01/10/2014"}</v>
       </c>
     </row>
@@ -3347,40 +3387,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q22" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/cLDBbZmS/MITX.png"</v>
+      </c>
+      <c r="R22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/cLDBbZmS/MITX.png"</v>
-      </c>
-      <c r="R22" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C22)</f>
         <v>category:"Education"</v>
       </c>
       <c r="S22" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D22)</f>
+        <f t="shared" si="2"/>
         <v>name:"Supply chain fundamentals"</v>
       </c>
       <c r="T22" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E22)</f>
+        <f t="shared" si="3"/>
         <v>location:"online"</v>
       </c>
       <c r="U22" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F22)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"MITx"</v>
       </c>
       <c r="V22" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I22)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"Excel tools from demand planning to CSL and sales evaluations"</v>
       </c>
       <c r="W22" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/05/2016"</v>
       </c>
       <c r="X22" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/07/2016"</v>
       </c>
       <c r="Y22" s="4"/>
       <c r="Z22" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/cLDBbZmS/MITX.png",category:"Education",name:"Supply chain fundamentals",location:"online",businessName:"MITx",jobDescription:"Excel tools from demand planning to CSL and sales evaluations","begin":"01/05/2016","end":"01/07/2016"}</v>
       </c>
     </row>
@@ -3429,40 +3469,40 @@
         <v>language:"ENG"</v>
       </c>
       <c r="Q23" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>image:"https://i.postimg.cc/QMt08VtC/ADELAIDE.png"</v>
+      </c>
+      <c r="R23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>image:"https://i.postimg.cc/QMt08VtC/ADELAIDE.png"</v>
-      </c>
-      <c r="R23" s="4" t="str">
-        <f>CONCATENATE(C$1,$R$1,C23)</f>
         <v>category:"Education"</v>
       </c>
       <c r="S23" s="4" t="str">
-        <f>CONCATENATE(D$1,$R$1,D23)</f>
+        <f t="shared" si="2"/>
         <v>name:"Project Management"</v>
       </c>
       <c r="T23" s="4" t="str">
-        <f>CONCATENATE(E$1,$R$1,E23)</f>
+        <f t="shared" si="3"/>
         <v>location:"online"</v>
       </c>
       <c r="U23" s="4" t="str">
-        <f>CONCATENATE(F$1,$R$1,F23)</f>
+        <f t="shared" si="4"/>
         <v>businessName:"AldeideX"</v>
       </c>
       <c r="V23" s="4" t="str">
-        <f>CONCATENATE(I$1,$R$1,I23)</f>
+        <f t="shared" si="5"/>
         <v>jobDescription:"3 months basic course in project management BOK"</v>
       </c>
       <c r="W23" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>"begin":"01/04/2016"</v>
       </c>
       <c r="X23" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>"end":"01/04/2016"</v>
       </c>
       <c r="Y23" s="4"/>
       <c r="Z23" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>{language:"ENG",image:"https://i.postimg.cc/QMt08VtC/ADELAIDE.png",category:"Education",name:"Project Management",location:"online",businessName:"AldeideX",jobDescription:"3 months basic course in project management BOK","begin":"01/04/2016","end":"01/04/2016"}</v>
       </c>
     </row>
@@ -3507,44 +3547,44 @@
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4" t="str">
-        <f t="shared" ref="P24:P27" si="5">CONCATENATE(A$1,$R$1,A24)</f>
+        <f t="shared" ref="P24:P27" si="10">CONCATENATE(A$1,$R$1,A24)</f>
         <v>language:"ENG"</v>
       </c>
       <c r="Q24" s="4" t="str">
-        <f t="shared" ref="Q24:Q27" si="6">CONCATENATE(B$1,$R$1,$T$1,B24,$T$1)</f>
+        <f t="shared" ref="Q24:Q27" si="11">CONCATENATE(B$1,$R$1,$T$1,B24,$T$1)</f>
         <v>image:"'https://i.postimg.cc/59vpNhxB/DBGA.png'"</v>
       </c>
       <c r="R24" s="4" t="str">
-        <f t="shared" ref="R24:R27" si="7">CONCATENATE(C$1,$R$1,C24)</f>
+        <f t="shared" ref="R24:R27" si="12">CONCATENATE(C$1,$R$1,C24)</f>
         <v>category:'Projects'</v>
       </c>
       <c r="S24" s="4" t="str">
-        <f t="shared" ref="S24:S27" si="8">CONCATENATE(D$1,$R$1,D24)</f>
+        <f t="shared" ref="S24:S27" si="13">CONCATENATE(D$1,$R$1,D24)</f>
         <v>name:'Weight control'</v>
       </c>
       <c r="T24" s="4" t="str">
-        <f t="shared" ref="T24:T27" si="9">CONCATENATE(E$1,$R$1,E24)</f>
+        <f t="shared" ref="T24:T27" si="14">CONCATENATE(E$1,$R$1,E24)</f>
         <v>location:'CDMX'</v>
       </c>
       <c r="U24" s="4" t="str">
-        <f t="shared" ref="U24:U27" si="10">CONCATENATE(F$1,$R$1,F24)</f>
+        <f t="shared" ref="U24:U27" si="15">CONCATENATE(F$1,$R$1,F24)</f>
         <v>businessName:'Personal'</v>
       </c>
       <c r="V24" s="4" t="str">
-        <f t="shared" ref="V24:V27" si="11">CONCATENATE(I$1,$R$1,I24)</f>
+        <f t="shared" ref="V24:V27" si="16">CONCATENATE(I$1,$R$1,I24)</f>
         <v>jobDescription:'lost 20 kg in 2 years'</v>
       </c>
       <c r="W24" s="4" t="str">
-        <f t="shared" ref="W24:W27" si="12">CONCATENATE(L$1,$R$1,$T$1,L24,$T$1)</f>
+        <f t="shared" ref="W24:W27" si="17">CONCATENATE(L$1,$R$1,$T$1,L24,$T$1)</f>
         <v>"begin":"13/02/2018"</v>
       </c>
       <c r="X24" s="4" t="str">
-        <f t="shared" ref="X24:X27" si="13">CONCATENATE(M$1,$R$1,$T$1,M24,$T$1)</f>
+        <f t="shared" ref="X24:X27" si="18">CONCATENATE(M$1,$R$1,$T$1,M24,$T$1)</f>
         <v>"end":"43917"</v>
       </c>
       <c r="Y24" s="4"/>
       <c r="Z24" s="4" t="str">
-        <f t="shared" ref="Z24:Z27" si="14">CONCATENATE($P$1,P24,$S$1,Q24,$S$1,R24,$S$1,S24,$S$1,T24,$S$1,U24,$S$1,V24,$S$1,W24,$S$1,X24,$Q$1)</f>
+        <f t="shared" ref="Z24:Z27" si="19">CONCATENATE($P$1,P24,$S$1,Q24,$S$1,R24,$S$1,S24,$S$1,T24,$S$1,U24,$S$1,V24,$S$1,W24,$S$1,X24,$Q$1)</f>
         <v>{language:"ENG",image:"'https://i.postimg.cc/59vpNhxB/DBGA.png'",category:'Projects',name:'Weight control',location:'CDMX',businessName:'Personal',jobDescription:'lost 20 kg in 2 years',"begin":"13/02/2018","end":"43917"}</v>
       </c>
     </row>
@@ -3589,44 +3629,44 @@
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>language:"ENG"</v>
       </c>
       <c r="Q25" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>image:"'https://i.postimg.cc/287wnnL3/HDGD.jpg'"</v>
       </c>
       <c r="R25" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>category:'Hobbies'</v>
       </c>
       <c r="S25" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>name:'Haidong Gumdo'</v>
       </c>
       <c r="T25" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>location:'CDMX'</v>
       </c>
       <c r="U25" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>businessName:'Haidong Gumdo'</v>
       </c>
       <c r="V25" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>jobDescription:'Korean martial art build around the use of swords'</v>
       </c>
       <c r="W25" s="4" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>"begin":"10/09/2005"</v>
       </c>
       <c r="X25" s="4" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>"end":"41104"</v>
       </c>
       <c r="Y25" s="4"/>
       <c r="Z25" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>{language:"ENG",image:"'https://i.postimg.cc/287wnnL3/HDGD.jpg'",category:'Hobbies',name:'Haidong Gumdo',location:'CDMX',businessName:'Haidong Gumdo',jobDescription:'Korean martial art build around the use of swords',"begin":"10/09/2005","end":"41104"}</v>
       </c>
     </row>
@@ -3671,44 +3711,44 @@
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>language:"ENG"</v>
       </c>
       <c r="Q26" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>image:"'https://i.postimg.cc/fR58QYM1/BMW.png'"</v>
       </c>
       <c r="R26" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>category:'Hobbies'</v>
       </c>
       <c r="S26" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>name:'Riding Motorcycle'</v>
       </c>
       <c r="T26" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>location:'multiple'</v>
       </c>
       <c r="U26" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>businessName:'BMW'</v>
       </c>
       <c r="V26" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>jobDescription:'Motorcycle riding and travels'</v>
       </c>
       <c r="W26" s="4" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>"begin":"02/03/2015"</v>
       </c>
       <c r="X26" s="4" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>"end":"44271"</v>
       </c>
       <c r="Y26" s="4"/>
       <c r="Z26" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>{language:"ENG",image:"'https://i.postimg.cc/fR58QYM1/BMW.png'",category:'Hobbies',name:'Riding Motorcycle',location:'multiple',businessName:'BMW',jobDescription:'Motorcycle riding and travels',"begin":"02/03/2015","end":"44271"}</v>
       </c>
     </row>
@@ -3751,44 +3791,44 @@
         <v>50</v>
       </c>
       <c r="P27" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>language:"ENG"</v>
       </c>
       <c r="Q27" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>image:"'https://i.postimg.cc/1z2cyH27/RAPAX.png'"</v>
       </c>
       <c r="R27" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>category:'Hobbies'</v>
       </c>
       <c r="S27" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>name:'Airsoft'</v>
       </c>
       <c r="T27" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>location:'multiple'</v>
       </c>
       <c r="U27" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>businessName:'LEGION RAPAX'</v>
       </c>
       <c r="V27" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>jobDescription:'Military simulations similar to gotcha, played since 2010, led team since 2017'</v>
       </c>
       <c r="W27" s="4" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>"begin":"02/06/2010"</v>
       </c>
       <c r="X27" s="4" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>"end":"current"</v>
       </c>
       <c r="Y27" s="4"/>
       <c r="Z27" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>{language:"ENG",image:"'https://i.postimg.cc/1z2cyH27/RAPAX.png'",category:'Hobbies',name:'Airsoft',location:'multiple',businessName:'LEGION RAPAX',jobDescription:'Military simulations similar to gotcha, played since 2010, led team since 2017',"begin":"02/06/2010","end":"current"}</v>
       </c>
     </row>
@@ -3819,13 +3859,13 @@
       <c r="Z29" s="4"/>
     </row>
     <row r="37" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="10" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>346</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -3833,8 +3873,8 @@
       <c r="M40" s="3"/>
     </row>
     <row r="41" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
-        <v>348</v>
+      <c r="A41" s="10" t="s">
+        <v>347</v>
       </c>
       <c r="L41" s="2"/>
       <c r="M41" s="3"/>
@@ -3844,118 +3884,544 @@
       <c r="M42" s="3"/>
     </row>
     <row r="43" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="45" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="45" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+    </row>
+    <row r="47" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
+    </row>
+    <row r="50" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-    </row>
-    <row r="50" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+    <row r="52" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+    <row r="54" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+    <row r="56" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+    <row r="58" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
+    <row r="62" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="11"/>
+    </row>
+    <row r="67" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
-    </row>
-    <row r="67" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="15" t="s">
+    <row r="69" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
+    <row r="71" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+    <row r="73" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
+    <row r="77" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="11"/>
+    </row>
+    <row r="84" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A84" s="10"/>
+    </row>
+    <row r="86" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A86" s="10"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="15" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="15" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="16"/>
-    </row>
-    <row r="84" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="15"/>
-    </row>
-    <row r="86" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
-    </row>
-    <row r="88" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A88" s="15"/>
+      <c r="B88" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C88" t="str">
+        <f>A88</f>
+        <v>Language</v>
+      </c>
+      <c r="D88" t="s">
+        <v>378</v>
+      </c>
+      <c r="E88" t="str">
+        <f>A88</f>
+        <v>Language</v>
+      </c>
+      <c r="F88" t="s">
+        <v>379</v>
+      </c>
+      <c r="G88" t="str">
+        <f>A88</f>
+        <v>Language</v>
+      </c>
+      <c r="H88" t="s">
+        <v>380</v>
+      </c>
+      <c r="I88" t="str">
+        <f>CONCATENATE(B88,C88,D88,E88,F88,G88,H88)</f>
+        <v>&lt;label&gt;Language:&lt;/label&gt;&lt;input name="Language value={this.state.timeline.Language} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" ref="C89:C100" si="20">A89</f>
+        <v>Image</v>
+      </c>
+      <c r="D89" t="s">
+        <v>378</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" ref="E89:E100" si="21">A89</f>
+        <v>Image</v>
+      </c>
+      <c r="F89" t="s">
+        <v>379</v>
+      </c>
+      <c r="G89" t="str">
+        <f t="shared" ref="G89:G100" si="22">A89</f>
+        <v>Image</v>
+      </c>
+      <c r="H89" t="s">
+        <v>380</v>
+      </c>
+      <c r="I89" t="str">
+        <f t="shared" ref="I89:I100" si="23">CONCATENATE(B89,C89,D89,E89,F89,G89,H89)</f>
+        <v>&lt;label&gt;Image:&lt;/label&gt;&lt;input name="Image value={this.state.timeline.Image} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="20"/>
+        <v>Category</v>
+      </c>
+      <c r="D90" t="s">
+        <v>378</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="21"/>
+        <v>Category</v>
+      </c>
+      <c r="F90" t="s">
+        <v>379</v>
+      </c>
+      <c r="G90" t="str">
+        <f t="shared" si="22"/>
+        <v>Category</v>
+      </c>
+      <c r="H90" t="s">
+        <v>380</v>
+      </c>
+      <c r="I90" t="str">
+        <f t="shared" si="23"/>
+        <v>&lt;label&gt;Category:&lt;/label&gt;&lt;input name="Category value={this.state.timeline.Category} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="20"/>
+        <v>Name</v>
+      </c>
+      <c r="D91" t="s">
+        <v>378</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="21"/>
+        <v>Name</v>
+      </c>
+      <c r="F91" t="s">
+        <v>379</v>
+      </c>
+      <c r="G91" t="str">
+        <f t="shared" si="22"/>
+        <v>Name</v>
+      </c>
+      <c r="H91" t="s">
+        <v>380</v>
+      </c>
+      <c r="I91" t="str">
+        <f t="shared" si="23"/>
+        <v>&lt;label&gt;Name:&lt;/label&gt;&lt;input name="Name value={this.state.timeline.Name} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="20"/>
+        <v>Location</v>
+      </c>
+      <c r="D92" t="s">
+        <v>378</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="21"/>
+        <v>Location</v>
+      </c>
+      <c r="F92" t="s">
+        <v>379</v>
+      </c>
+      <c r="G92" t="str">
+        <f t="shared" si="22"/>
+        <v>Location</v>
+      </c>
+      <c r="H92" t="s">
+        <v>380</v>
+      </c>
+      <c r="I92" t="str">
+        <f t="shared" si="23"/>
+        <v>&lt;label&gt;Location:&lt;/label&gt;&lt;input name="Location value={this.state.timeline.Location} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="20"/>
+        <v>BusinessName</v>
+      </c>
+      <c r="D93" t="s">
+        <v>378</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="21"/>
+        <v>BusinessName</v>
+      </c>
+      <c r="F93" t="s">
+        <v>379</v>
+      </c>
+      <c r="G93" t="str">
+        <f t="shared" si="22"/>
+        <v>BusinessName</v>
+      </c>
+      <c r="H93" t="s">
+        <v>380</v>
+      </c>
+      <c r="I93" t="str">
+        <f t="shared" si="23"/>
+        <v>&lt;label&gt;BusinessName:&lt;/label&gt;&lt;input name="BusinessName value={this.state.timeline.BusinessName} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="20"/>
+        <v>Skills</v>
+      </c>
+      <c r="D94" t="s">
+        <v>378</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="21"/>
+        <v>Skills</v>
+      </c>
+      <c r="F94" t="s">
+        <v>379</v>
+      </c>
+      <c r="G94" t="str">
+        <f t="shared" si="22"/>
+        <v>Skills</v>
+      </c>
+      <c r="H94" t="s">
+        <v>380</v>
+      </c>
+      <c r="I94" t="str">
+        <f t="shared" si="23"/>
+        <v>&lt;label&gt;Skills:&lt;/label&gt;&lt;input name="Skills value={this.state.timeline.Skills} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="20"/>
+        <v>BusinessDescription</v>
+      </c>
+      <c r="D95" t="s">
+        <v>378</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="21"/>
+        <v>BusinessDescription</v>
+      </c>
+      <c r="F95" t="s">
+        <v>379</v>
+      </c>
+      <c r="G95" t="str">
+        <f t="shared" si="22"/>
+        <v>BusinessDescription</v>
+      </c>
+      <c r="H95" t="s">
+        <v>380</v>
+      </c>
+      <c r="I95" t="str">
+        <f t="shared" si="23"/>
+        <v>&lt;label&gt;BusinessDescription:&lt;/label&gt;&lt;input name="BusinessDescription value={this.state.timeline.BusinessDescription} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="20"/>
+        <v>JobDescription</v>
+      </c>
+      <c r="D96" t="s">
+        <v>378</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="21"/>
+        <v>JobDescription</v>
+      </c>
+      <c r="F96" t="s">
+        <v>379</v>
+      </c>
+      <c r="G96" t="str">
+        <f t="shared" si="22"/>
+        <v>JobDescription</v>
+      </c>
+      <c r="H96" t="s">
+        <v>380</v>
+      </c>
+      <c r="I96" t="str">
+        <f t="shared" si="23"/>
+        <v>&lt;label&gt;JobDescription:&lt;/label&gt;&lt;input name="JobDescription value={this.state.timeline.JobDescription} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="20"/>
+        <v>Schedule</v>
+      </c>
+      <c r="D97" t="s">
+        <v>378</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="21"/>
+        <v>Schedule</v>
+      </c>
+      <c r="F97" t="s">
+        <v>379</v>
+      </c>
+      <c r="G97" t="str">
+        <f t="shared" si="22"/>
+        <v>Schedule</v>
+      </c>
+      <c r="H97" t="s">
+        <v>380</v>
+      </c>
+      <c r="I97" t="str">
+        <f t="shared" si="23"/>
+        <v>&lt;label&gt;Schedule:&lt;/label&gt;&lt;input name="Schedule value={this.state.timeline.Schedule} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="20"/>
+        <v>WorkTime</v>
+      </c>
+      <c r="D98" t="s">
+        <v>378</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="21"/>
+        <v>WorkTime</v>
+      </c>
+      <c r="F98" t="s">
+        <v>379</v>
+      </c>
+      <c r="G98" t="str">
+        <f t="shared" si="22"/>
+        <v>WorkTime</v>
+      </c>
+      <c r="H98" t="s">
+        <v>380</v>
+      </c>
+      <c r="I98" t="str">
+        <f t="shared" si="23"/>
+        <v>&lt;label&gt;WorkTime:&lt;/label&gt;&lt;input name="WorkTime value={this.state.timeline.WorkTime} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="20"/>
+        <v>Begin</v>
+      </c>
+      <c r="D99" t="s">
+        <v>378</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="21"/>
+        <v>Begin</v>
+      </c>
+      <c r="F99" t="s">
+        <v>379</v>
+      </c>
+      <c r="G99" t="str">
+        <f t="shared" si="22"/>
+        <v>Begin</v>
+      </c>
+      <c r="H99" t="s">
+        <v>380</v>
+      </c>
+      <c r="I99" t="str">
+        <f t="shared" si="23"/>
+        <v>&lt;label&gt;Begin:&lt;/label&gt;&lt;input name="Begin value={this.state.timeline.Begin} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="20"/>
+        <v>End</v>
+      </c>
+      <c r="D100" t="s">
+        <v>378</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="21"/>
+        <v>End</v>
+      </c>
+      <c r="F100" t="s">
+        <v>379</v>
+      </c>
+      <c r="G100" t="str">
+        <f t="shared" si="22"/>
+        <v>End</v>
+      </c>
+      <c r="H100" t="s">
+        <v>380</v>
+      </c>
+      <c r="I100" t="str">
+        <f t="shared" si="23"/>
+        <v>&lt;label&gt;End:&lt;/label&gt;&lt;input name="End value={this.state.timeline.End} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3989,14 +4455,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACBE0D3-1FED-444E-85F3-AC56CB93C951}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="I20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4019,733 +4484,733 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="4" t="s">
         <v>262</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="O3" s="4" t="s">
         <v>260</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="O4" s="4" t="s">
         <v>259</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="3"/>
     </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="M5" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="4" t="s">
         <v>258</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="M6" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="4" t="s">
         <v>261</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="N7" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="O7" s="4" t="s">
         <v>250</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="M8" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="N8" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="O8" s="4" t="s">
         <v>251</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="M9" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" s="4" t="s">
         <v>252</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="L10" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="M10" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="N10" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="O10" s="4" t="s">
         <v>253</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="L11" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="M11" s="9" t="s">
+      <c r="M11" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="N11" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="O11" s="4" t="s">
         <v>255</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L12" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="M12" s="9" t="s">
+      <c r="M12" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="N12" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="O12" s="4" t="s">
         <v>256</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="L13" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M13" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="N13" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="O13" s="4" t="s">
         <v>254</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="L14" s="9" t="s">
+      <c r="L14" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="M14" s="9" t="s">
+      <c r="M14" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="N14" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="O14" s="4" t="s">
         <v>257</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="3"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="M15" s="9" t="s">
+      <c r="M15" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="N15" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="O15" s="9" t="s">
+      <c r="O15" s="4" t="s">
         <v>263</v>
       </c>
       <c r="Q15" s="2"/>
@@ -4754,15 +5219,443 @@
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C21" t="str">
+        <f>A21</f>
+        <v>Langauge</v>
+      </c>
+      <c r="D21" t="s">
+        <v>378</v>
+      </c>
+      <c r="E21" t="str">
+        <f>A21</f>
+        <v>Langauge</v>
+      </c>
+      <c r="F21" t="s">
+        <v>387</v>
+      </c>
+      <c r="G21" t="str">
+        <f>A21</f>
+        <v>Langauge</v>
+      </c>
+      <c r="H21" t="s">
+        <v>380</v>
+      </c>
+      <c r="I21" t="str">
+        <f>CONCATENATE(B21,C21,D21,E21,F21,G21,H21)</f>
+        <v>&lt;label&gt;Langauge:&lt;/label&gt;&lt;input name="Langauge value={this.state.article.Langauge} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" ref="C22:C33" si="0">A22</f>
+        <v>Title</v>
+      </c>
+      <c r="D22" t="s">
+        <v>378</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" ref="E22:E33" si="1">A22</f>
+        <v>Title</v>
+      </c>
+      <c r="F22" t="s">
+        <v>387</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" ref="G22:G33" si="2">A22</f>
+        <v>Title</v>
+      </c>
+      <c r="H22" t="s">
+        <v>380</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" ref="I22:I33" si="3">CONCATENATE(B22,C22,D22,E22,F22,G22,H22)</f>
+        <v>&lt;label&gt;Title:&lt;/label&gt;&lt;input name="Title value={this.state.article.Title} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>Education</v>
+      </c>
+      <c r="D23" t="s">
+        <v>378</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>Education</v>
+      </c>
+      <c r="F23" t="s">
+        <v>387</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>Education</v>
+      </c>
+      <c r="H23" t="s">
+        <v>380</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;label&gt;Education:&lt;/label&gt;&lt;input name="Education value={this.state.article.Education} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>Work</v>
+      </c>
+      <c r="D24" t="s">
+        <v>378</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>Work</v>
+      </c>
+      <c r="F24" t="s">
+        <v>387</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>Work</v>
+      </c>
+      <c r="H24" t="s">
+        <v>380</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;label&gt;Work:&lt;/label&gt;&lt;input name="Work value={this.state.article.Work} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Location</v>
+      </c>
+      <c r="D25" t="s">
+        <v>378</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>Location</v>
+      </c>
+      <c r="F25" t="s">
+        <v>387</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>Location</v>
+      </c>
+      <c r="H25" t="s">
+        <v>380</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;label&gt;Location:&lt;/label&gt;&lt;input name="Location value={this.state.article.Location} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>Logo</v>
+      </c>
+      <c r="D26" t="s">
+        <v>378</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>Logo</v>
+      </c>
+      <c r="F26" t="s">
+        <v>387</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>Logo</v>
+      </c>
+      <c r="H26" t="s">
+        <v>380</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;label&gt;Logo:&lt;/label&gt;&lt;input name="Logo value={this.state.article.Logo} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>ShortDescription</v>
+      </c>
+      <c r="D27" t="s">
+        <v>378</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>ShortDescription</v>
+      </c>
+      <c r="F27" t="s">
+        <v>387</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>ShortDescription</v>
+      </c>
+      <c r="H27" t="s">
+        <v>380</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;label&gt;ShortDescription:&lt;/label&gt;&lt;input name="ShortDescription value={this.state.article.ShortDescription} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>ProblemDescription</v>
+      </c>
+      <c r="D28" t="s">
+        <v>378</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>ProblemDescription</v>
+      </c>
+      <c r="F28" t="s">
+        <v>387</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>ProblemDescription</v>
+      </c>
+      <c r="H28" t="s">
+        <v>380</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;label&gt;ProblemDescription:&lt;/label&gt;&lt;input name="ProblemDescription value={this.state.article.ProblemDescription} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>DesiredState</v>
+      </c>
+      <c r="D29" t="s">
+        <v>378</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>DesiredState</v>
+      </c>
+      <c r="F29" t="s">
+        <v>387</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>DesiredState</v>
+      </c>
+      <c r="H29" t="s">
+        <v>380</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;label&gt;DesiredState:&lt;/label&gt;&lt;input name="DesiredState value={this.state.article.DesiredState} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>Goals</v>
+      </c>
+      <c r="D30" t="s">
+        <v>378</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>Goals</v>
+      </c>
+      <c r="F30" t="s">
+        <v>387</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>Goals</v>
+      </c>
+      <c r="H30" t="s">
+        <v>380</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;label&gt;Goals:&lt;/label&gt;&lt;input name="Goals value={this.state.article.Goals} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>TimeConstraints</v>
+      </c>
+      <c r="D31" t="s">
+        <v>378</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>TimeConstraints</v>
+      </c>
+      <c r="F31" t="s">
+        <v>387</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>TimeConstraints</v>
+      </c>
+      <c r="H31" t="s">
+        <v>380</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;label&gt;TimeConstraints:&lt;/label&gt;&lt;input name="TimeConstraints value={this.state.article.TimeConstraints} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>Plan</v>
+      </c>
+      <c r="D32" t="s">
+        <v>378</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>Plan</v>
+      </c>
+      <c r="F32" t="s">
+        <v>387</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>Plan</v>
+      </c>
+      <c r="H32" t="s">
+        <v>380</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;label&gt;Plan:&lt;/label&gt;&lt;input name="Plan value={this.state.article.Plan} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>Tools</v>
+      </c>
+      <c r="D33" t="s">
+        <v>378</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>Tools</v>
+      </c>
+      <c r="F33" t="s">
+        <v>387</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>Tools</v>
+      </c>
+      <c r="H33" t="s">
+        <v>380</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="3"/>
+        <v>&lt;label&gt;Tools:&lt;/label&gt;&lt;input name="Tools value={this.state.article.Tools} type=text" onChange={(e)=&gt; this.handleChange(e.target.name, e.target.value)} /&gt;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O15" xr:uid="{DACBE0D3-1FED-444E-85F3-AC56CB93C951}">
-    <filterColumn colId="0">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O15">
-      <sortCondition sortBy="cellColor" ref="A1:A15" dxfId="1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:O15" xr:uid="{DACBE0D3-1FED-444E-85F3-AC56CB93C951}"/>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{D5AB55C9-B0E6-4294-820E-7264AD3AC4A9}"/>
     <hyperlink ref="F7" r:id="rId2" xr:uid="{DAD769E2-F919-46EA-9826-4A3A95094776}"/>

</xml_diff>

<commit_message>
fixing problems with lenguage selector
</commit_message>
<xml_diff>
--- a/src/recursos/BDD Timeline.xlsx
+++ b/src/recursos/BDD Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Files\Programming\portfolio\src\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77129F3-F1FF-4DA8-979D-9052C1872827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8E6949-A62D-4426-93FE-915F6AA8D2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
+    <workbookView xWindow="10245" yWindow="0" windowWidth="10215" windowHeight="10920" activeTab="2" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
   </bookViews>
   <sheets>
     <sheet name="display" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="define fields" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">articles!$A$1:$P$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">articles!$A$1:$Q$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'work exp'!$A$1:$M$18</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="564">
   <si>
     <t>Location</t>
   </si>
@@ -1361,9 +1361,6 @@
     <t>Control de negocio</t>
   </si>
   <si>
-    <t>Historial de compras</t>
-  </si>
-  <si>
     <t>Herramienta de control de presupuesto</t>
   </si>
   <si>
@@ -1821,6 +1818,12 @@
   </si>
   <si>
     <t>["Diseñar actividades de airsoft económicas pero entretenidas","Asegurar un lugar para el evento","Crear una invitación","Enviarla a tantos airsofters como sea posible","Comandar y controlar el evento","Entregar los fondos a Aníbal","Enviar evidencia de pago a los equipos de airsoft para garantizar transparencia"]</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Historial de ventas</t>
   </si>
 </sst>
 </file>
@@ -1929,7 +1932,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1955,8 +1958,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1965,74 +1973,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2049,10 +1989,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2652,9 +2592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08630837-D9DA-4E92-997A-E80AD53DE965}">
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H12" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4175,1544 +4113,1638 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACBE0D3-1FED-444E-85F3-AC56CB93C951}">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P29" sqref="P29"/>
+      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="83" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="114.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="131" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="189.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="96.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="53" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="53" customWidth="1"/>
-    <col min="16" max="16" width="144" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="83" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="114.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="131" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="189.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="96.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="53" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="53" customWidth="1"/>
+    <col min="17" max="17" width="144" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>422</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>457</v>
+        <v>421</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>488</v>
+        <v>456</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>521</v>
+        <v>487</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="3"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S2" s="2"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>49</v>
+        <v>243</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>407</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>423</v>
-      </c>
       <c r="H3" s="4" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>489</v>
+        <v>470</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>522</v>
+        <v>501</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>92</v>
+        <v>533</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>204</v>
+        <v>449</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>545</v>
       </c>
       <c r="N3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="P3" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="R3" s="2"/>
-      <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="S3" s="2"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>97</v>
+      <c r="B4" s="4">
+        <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>424</v>
+        <v>62</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>459</v>
+        <v>422</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>490</v>
+        <v>457</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>523</v>
+        <v>488</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>82</v>
+        <v>521</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="N4" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O4" s="9" t="s">
-        <v>124</v>
-      </c>
       <c r="P4" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="3"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="S4" s="2"/>
+      <c r="T4" s="3"/>
+    </row>
+    <row r="5" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>243</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>408</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>51</v>
+        <v>418</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>425</v>
+      <c r="G5" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>460</v>
+        <v>435</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>491</v>
+        <v>471</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>524</v>
+        <v>502</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>82</v>
+        <v>534</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>94</v>
+        <v>450</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>546</v>
       </c>
       <c r="N5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O5" s="9" t="s">
-        <v>115</v>
-      </c>
       <c r="P5" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="R5" s="2"/>
-      <c r="S5" s="3"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="S5" s="2"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>55</v>
+      <c r="B6" s="4">
+        <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>229</v>
+        <v>97</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>426</v>
+        <v>61</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>461</v>
+        <v>423</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>492</v>
+        <v>458</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>520</v>
+        <v>489</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>78</v>
+        <v>522</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>552</v>
+        <v>82</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>79</v>
+        <v>135</v>
       </c>
       <c r="N6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O6" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="R6" s="2"/>
-      <c r="S6" s="3"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="P6" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="S6" s="2"/>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="17">
+        <v>3</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>436</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>472</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>503</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>535</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>451</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q7" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="S7" s="2"/>
+      <c r="T7" s="3"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>427</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>462</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>525</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>551</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="N7" s="4" t="s">
+      <c r="B8" s="17">
+        <v>4</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>428</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>463</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>494</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>526</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>554</v>
+      </c>
+      <c r="N8" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="O8" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="R7" s="2"/>
-      <c r="S7" s="3"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>526</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="N8" s="4" t="s">
+      <c r="P8" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q8" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="S8" s="2"/>
+      <c r="T8" s="3"/>
+    </row>
+    <row r="9" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9" s="4">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>556</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O8" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="R8" s="2"/>
-      <c r="S8" s="3"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>464</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>495</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O9" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="R9" s="2"/>
-      <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S9" s="2"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="4">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>430</v>
-      </c>
       <c r="H10" s="4" t="s">
-        <v>465</v>
+        <v>429</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>496</v>
+        <v>464</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>528</v>
+        <v>495</v>
       </c>
       <c r="K10" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="M10" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="N10" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="O10" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="P10" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="R10" s="2"/>
-      <c r="S10" s="3"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S10" s="2"/>
+      <c r="T10" s="3"/>
+    </row>
+    <row r="11" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>52</v>
+        <v>243</v>
+      </c>
+      <c r="B11" s="4">
+        <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>53</v>
+        <v>413</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>431</v>
+        <v>419</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>497</v>
+        <v>478</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>529</v>
+        <v>509</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>86</v>
+        <v>516</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>89</v>
+        <v>454</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>555</v>
       </c>
       <c r="N11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O11" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O11" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="P11" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="R11" s="2"/>
-      <c r="S11" s="3"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="T11" s="3"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>56</v>
+      <c r="B12" s="4">
+        <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>432</v>
+        <v>64</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>467</v>
+        <v>427</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>498</v>
+        <v>462</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>530</v>
+        <v>493</v>
       </c>
       <c r="K12" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="L12" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="M12" s="4" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="N12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O12" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O12" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="P12" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="R12" s="2"/>
-      <c r="S12" s="3"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="S12" s="2"/>
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>57</v>
+        <v>243</v>
+      </c>
+      <c r="B13" s="4">
+        <v>6</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>49</v>
+        <v>411</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>51</v>
+        <v>418</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>433</v>
+        <v>64</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>468</v>
+        <v>440</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>499</v>
+        <v>476</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>531</v>
+        <v>507</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>88</v>
+        <v>514</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>96</v>
+        <v>451</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>553</v>
       </c>
       <c r="N13" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="O13" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O13" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="P13" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="R13" s="2"/>
-      <c r="S13" s="3"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="S13" s="2"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>139</v>
+      <c r="B14" s="4">
+        <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>51</v>
+        <v>229</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="S14" s="2"/>
+      <c r="T14" s="3"/>
+    </row>
+    <row r="15" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="17">
+        <v>7</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>420</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>474</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>505</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>452</v>
+      </c>
+      <c r="M15" s="20" t="s">
+        <v>549</v>
+      </c>
+      <c r="N15" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="O15" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="P15" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q15" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="S15" s="2"/>
+      <c r="T15" s="3"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="4">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>434</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="G16" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="J16" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="L16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="L14" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="N14" s="4" t="s">
+      <c r="M16" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O14" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="R14" s="2"/>
-      <c r="S14" s="3"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>470</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>533</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O15" s="4" t="s">
+      <c r="P16" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="Q16" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="3"/>
-    </row>
-    <row r="16" spans="1:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>471</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>502</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>450</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>546</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>408</v>
+      <c r="B17" s="4">
+        <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>419</v>
+        <v>99</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>62</v>
+        <v>418</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>436</v>
+      <c r="G17" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>472</v>
+        <v>447</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>503</v>
+        <v>483</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>535</v>
+        <v>511</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="L17" s="14" t="s">
-        <v>547</v>
-      </c>
-      <c r="M17" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="N17" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="O17" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O17" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="P17" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>409</v>
+        <v>54</v>
+      </c>
+      <c r="B18" s="4">
+        <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>419</v>
+        <v>230</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>61</v>
+        <v>229</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>437</v>
+        <v>63</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>473</v>
+        <v>426</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>504</v>
+        <v>461</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>536</v>
+        <v>492</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="L18" s="14" t="s">
-        <v>548</v>
+        <v>524</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>541</v>
+        <v>550</v>
       </c>
       <c r="N18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="O18" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O18" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="Q18" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="4">
+        <v>9</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="17">
+        <v>10</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F20" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G20" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>537</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="L19" s="14" t="s">
-        <v>549</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>542</v>
-      </c>
-      <c r="N19" s="4" t="s">
+      <c r="H20" s="17" t="s">
+        <v>424</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>459</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>490</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>523</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="N20" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="O20" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="O19" s="9" t="s">
+      <c r="P20" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="P19" s="4" t="s">
+      <c r="Q20" s="17" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>421</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="L20" s="14" t="s">
-        <v>550</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P20" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>411</v>
+      <c r="B21" s="4">
+        <v>10</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>63</v>
+        <v>419</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>440</v>
+      <c r="G21" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>507</v>
+        <v>473</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="L21" s="14" t="s">
-        <v>553</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>81</v>
+        <v>536</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="M21" s="14" t="s">
+        <v>548</v>
       </c>
       <c r="N21" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="O21" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P21" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="P21" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>412</v>
+        <v>54</v>
+      </c>
+      <c r="B22" s="4">
+        <v>11</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>419</v>
+        <v>52</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>477</v>
+        <v>51</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>430</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>508</v>
+        <v>465</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>515</v>
+        <v>496</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>554</v>
+        <v>528</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>543</v>
+        <v>130</v>
       </c>
       <c r="N22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="O22" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O22" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="P22" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>413</v>
+      <c r="B23" s="4">
+        <v>11</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="E23" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>442</v>
+        <v>51</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>478</v>
+        <v>443</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>516</v>
+        <v>484</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="L23" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="M23" s="14" t="s">
         <v>557</v>
       </c>
-      <c r="M23" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="N23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="O23" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O23" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="P23" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>510</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>517</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="L24" s="14" t="s">
-        <v>556</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="N24" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="17">
+        <v>12</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>431</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>497</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>529</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="M24" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="N24" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="O24" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="O24" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="P24" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="P24" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q24" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>415</v>
+      <c r="B25" s="4">
+        <v>12</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="I25" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>485</v>
-      </c>
       <c r="J25" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="K25" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="K25" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="L25" s="14" t="s">
+      <c r="L25" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="M25" s="14" t="s">
         <v>558</v>
       </c>
-      <c r="M25" s="4" t="s">
+      <c r="N25" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="N25" s="4" t="s">
+      <c r="O25" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O25" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="P25" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>418</v>
+        <v>54</v>
+      </c>
+      <c r="B26" s="4">
+        <v>13</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>419</v>
+        <v>57</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>481</v>
+      <c r="H26" s="6" t="s">
+        <v>432</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>511</v>
+        <v>467</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>519</v>
+        <v>498</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="L26" s="14" t="s">
-        <v>559</v>
+        <v>530</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="N26" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="O26" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O26" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="P26" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="40.5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="4">
+        <v>13</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="I27" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="J27" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="L27" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="L27" s="17" t="s">
+      <c r="M27" s="14" t="s">
         <v>560</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="N27" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="N27" s="4" t="s">
+      <c r="O27" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="O27" s="4" t="s">
+      <c r="P27" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="4">
+        <v>14</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="P28" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B29" s="17">
+        <v>14</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>415</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>445</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>481</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>485</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>454</v>
+      </c>
+      <c r="M29" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="N29" s="17" t="s">
+        <v>543</v>
+      </c>
+      <c r="O29" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="P29" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="P27" s="4" t="s">
+      <c r="Q29" s="17" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>539</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="L28" s="14" t="s">
-        <v>561</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>545</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="P28" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="L29" s="14" t="s">
-        <v>562</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O29" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="P29" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P15" xr:uid="{DACBE0D3-1FED-444E-85F3-AC56CB93C951}"/>
+  <autoFilter ref="A1:Q15" xr:uid="{DACBE0D3-1FED-444E-85F3-AC56CB93C951}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q29">
+      <sortCondition ref="B1:B15"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" xr:uid="{D5AB55C9-B0E6-4294-820E-7264AD3AC4A9}"/>
-    <hyperlink ref="F7" r:id="rId2" xr:uid="{DAD769E2-F919-46EA-9826-4A3A95094776}"/>
-    <hyperlink ref="F8" r:id="rId3" xr:uid="{DA58FBD3-A531-4FAF-A660-13EBE65967A4}"/>
-    <hyperlink ref="F9" r:id="rId4" xr:uid="{6DF98C11-E740-447A-BB1C-1A93B5A891DB}"/>
-    <hyperlink ref="F10" r:id="rId5" xr:uid="{306275F2-92C1-4503-BA0F-EDB80324B731}"/>
-    <hyperlink ref="F11" r:id="rId6" xr:uid="{CF9FCE47-D5A2-4D69-8C40-D4C64D534A8E}"/>
-    <hyperlink ref="F12" r:id="rId7" xr:uid="{2814EC2F-CE70-402C-8950-006DBF4E5E08}"/>
-    <hyperlink ref="F13" r:id="rId8" xr:uid="{1A842832-3FC2-48FE-B683-F5382A216B71}"/>
-    <hyperlink ref="F14" r:id="rId9" xr:uid="{AB31D706-35AD-460F-8E40-8BB54B871C4D}"/>
-    <hyperlink ref="F5" r:id="rId10" xr:uid="{B17BD6B2-73AB-45C4-B814-0452D99EB8CB}"/>
-    <hyperlink ref="F4" r:id="rId11" xr:uid="{DD09F1A0-7FA8-4A7E-83BC-E492F58B83A1}"/>
-    <hyperlink ref="F3" r:id="rId12" xr:uid="{763EB581-3C7F-4536-9511-C436874F6D99}"/>
-    <hyperlink ref="F15" r:id="rId13" xr:uid="{F8B839E1-8BE9-4F97-9DFB-B533A619B800}"/>
-    <hyperlink ref="F20" r:id="rId14" xr:uid="{D0FB9FA3-661D-42C8-BBD4-FF5DFBE70BEE}"/>
-    <hyperlink ref="F21" r:id="rId15" xr:uid="{69A35F35-B05F-48FC-8B27-2A6A9B526FC2}"/>
-    <hyperlink ref="F22" r:id="rId16" xr:uid="{16A15DDB-B8F3-4D74-A5F7-CEA2383554FD}"/>
-    <hyperlink ref="F23" r:id="rId17" xr:uid="{769F0F3F-54E9-4492-BBD6-DEB3699ADBC8}"/>
-    <hyperlink ref="F24" r:id="rId18" xr:uid="{325F1F83-D7FB-49D1-BAA6-A6AC8A591AB4}"/>
-    <hyperlink ref="F25" r:id="rId19" xr:uid="{C366C537-39A8-4FD1-9DF4-47D802C4D87B}"/>
-    <hyperlink ref="F26" r:id="rId20" xr:uid="{B25EBB74-92D4-42A3-B42C-093E7B8682FA}"/>
-    <hyperlink ref="F27" r:id="rId21" xr:uid="{8F63A4EC-77C0-4F49-A1BD-38313F58E8C7}"/>
-    <hyperlink ref="F28" r:id="rId22" xr:uid="{2F8E0850-7792-4D30-81ED-5F854ED0F245}"/>
-    <hyperlink ref="F19" r:id="rId23" xr:uid="{18692732-B7AF-46F4-BFC9-71A88827CDCF}"/>
-    <hyperlink ref="F18" r:id="rId24" xr:uid="{C1E8E182-0328-4425-9F38-80EAAFD5B23E}"/>
-    <hyperlink ref="F16" r:id="rId25" xr:uid="{35762721-F7DA-4140-8685-A6D12B734875}"/>
-    <hyperlink ref="F29" r:id="rId26" xr:uid="{3965A618-D2A1-4C20-AE39-9CA96872F9CF}"/>
-    <hyperlink ref="F2" r:id="rId27" xr:uid="{72CAF257-10DA-4E0D-BB2E-DC56256F4B95}"/>
-    <hyperlink ref="F17" r:id="rId28" xr:uid="{A76CAA92-FAD9-4B0A-BA85-B6A27F794D20}"/>
+    <hyperlink ref="G14" r:id="rId1" xr:uid="{D5AB55C9-B0E6-4294-820E-7264AD3AC4A9}"/>
+    <hyperlink ref="G18" r:id="rId2" xr:uid="{DAD769E2-F919-46EA-9826-4A3A95094776}"/>
+    <hyperlink ref="G12" r:id="rId3" xr:uid="{DA58FBD3-A531-4FAF-A660-13EBE65967A4}"/>
+    <hyperlink ref="G8" r:id="rId4" xr:uid="{6DF98C11-E740-447A-BB1C-1A93B5A891DB}"/>
+    <hyperlink ref="G10" r:id="rId5" xr:uid="{306275F2-92C1-4503-BA0F-EDB80324B731}"/>
+    <hyperlink ref="G22" r:id="rId6" xr:uid="{CF9FCE47-D5A2-4D69-8C40-D4C64D534A8E}"/>
+    <hyperlink ref="G24" r:id="rId7" xr:uid="{2814EC2F-CE70-402C-8950-006DBF4E5E08}"/>
+    <hyperlink ref="G26" r:id="rId8" xr:uid="{1A842832-3FC2-48FE-B683-F5382A216B71}"/>
+    <hyperlink ref="G28" r:id="rId9" xr:uid="{AB31D706-35AD-460F-8E40-8BB54B871C4D}"/>
+    <hyperlink ref="G20" r:id="rId10" xr:uid="{B17BD6B2-73AB-45C4-B814-0452D99EB8CB}"/>
+    <hyperlink ref="G6" r:id="rId11" xr:uid="{DD09F1A0-7FA8-4A7E-83BC-E492F58B83A1}"/>
+    <hyperlink ref="G4" r:id="rId12" xr:uid="{763EB581-3C7F-4536-9511-C436874F6D99}"/>
+    <hyperlink ref="G16" r:id="rId13" xr:uid="{F8B839E1-8BE9-4F97-9DFB-B533A619B800}"/>
+    <hyperlink ref="G15" r:id="rId14" xr:uid="{D0FB9FA3-661D-42C8-BBD4-FF5DFBE70BEE}"/>
+    <hyperlink ref="G19" r:id="rId15" xr:uid="{69A35F35-B05F-48FC-8B27-2A6A9B526FC2}"/>
+    <hyperlink ref="G13" r:id="rId16" xr:uid="{16A15DDB-B8F3-4D74-A5F7-CEA2383554FD}"/>
+    <hyperlink ref="G9" r:id="rId17" xr:uid="{769F0F3F-54E9-4492-BBD6-DEB3699ADBC8}"/>
+    <hyperlink ref="G11" r:id="rId18" xr:uid="{325F1F83-D7FB-49D1-BAA6-A6AC8A591AB4}"/>
+    <hyperlink ref="G23" r:id="rId19" xr:uid="{C366C537-39A8-4FD1-9DF4-47D802C4D87B}"/>
+    <hyperlink ref="G25" r:id="rId20" xr:uid="{B25EBB74-92D4-42A3-B42C-093E7B8682FA}"/>
+    <hyperlink ref="G29" r:id="rId21" xr:uid="{8F63A4EC-77C0-4F49-A1BD-38313F58E8C7}"/>
+    <hyperlink ref="G27" r:id="rId22" xr:uid="{2F8E0850-7792-4D30-81ED-5F854ED0F245}"/>
+    <hyperlink ref="G21" r:id="rId23" xr:uid="{18692732-B7AF-46F4-BFC9-71A88827CDCF}"/>
+    <hyperlink ref="G7" r:id="rId24" xr:uid="{C1E8E182-0328-4425-9F38-80EAAFD5B23E}"/>
+    <hyperlink ref="G3" r:id="rId25" xr:uid="{35762721-F7DA-4140-8685-A6D12B734875}"/>
+    <hyperlink ref="G17" r:id="rId26" xr:uid="{3965A618-D2A1-4C20-AE39-9CA96872F9CF}"/>
+    <hyperlink ref="G2" r:id="rId27" xr:uid="{72CAF257-10DA-4E0D-BB2E-DC56256F4B95}"/>
+    <hyperlink ref="G5" r:id="rId28" xr:uid="{A76CAA92-FAD9-4B0A-BA85-B6A27F794D20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId29"/>

</xml_diff>

<commit_message>
fixed all data errors
</commit_message>
<xml_diff>
--- a/src/recursos/BDD Timeline.xlsx
+++ b/src/recursos/BDD Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Files\Programming\portfolio\src\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8E6949-A62D-4426-93FE-915F6AA8D2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B00D2D6-D339-418E-A74C-9E0D761DB84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10215" windowHeight="10920" activeTab="2" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
   </bookViews>
   <sheets>
     <sheet name="display" sheetId="4" r:id="rId1"/>
@@ -1932,7 +1932,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1958,12 +1958,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4116,10 +4112,10 @@
   <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Q10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
+      <selection pane="bottomRight" activeCell="Q29" sqref="A29:Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4472,110 +4468,110 @@
       <c r="T6" s="3"/>
     </row>
     <row r="7" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="17" t="s">
         <v>547</v>
       </c>
-      <c r="N7" s="17" t="s">
+      <c r="N7" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="O7" s="17" t="s">
+      <c r="O7" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P7" s="19" t="s">
+      <c r="P7" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="Q7" s="17" t="s">
+      <c r="Q7" s="4" t="s">
         <v>110</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="3"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="M8" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="N8" s="17" t="s">
+      <c r="N8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="O8" s="17" t="s">
+      <c r="O8" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P8" s="17" t="s">
+      <c r="P8" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="Q8" s="17" t="s">
+      <c r="Q8" s="4" t="s">
         <v>103</v>
       </c>
       <c r="S8" s="2"/>
@@ -4912,55 +4908,55 @@
       <c r="T14" s="3"/>
     </row>
     <row r="15" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="4">
         <v>7</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="L15" s="17" t="s">
+      <c r="L15" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="M15" s="20" t="s">
+      <c r="M15" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="N15" s="17" t="s">
+      <c r="N15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="O15" s="17" t="s">
+      <c r="O15" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P15" s="17" t="s">
+      <c r="P15" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="Q15" s="17" t="s">
+      <c r="Q15" s="4" t="s">
         <v>112</v>
       </c>
       <c r="S15" s="2"/>
@@ -5173,55 +5169,55 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="4">
         <v>10</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="4" t="s">
         <v>459</v>
       </c>
-      <c r="J20" s="17" t="s">
+      <c r="J20" s="4" t="s">
         <v>490</v>
       </c>
-      <c r="K20" s="17" t="s">
+      <c r="K20" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="L20" s="17" t="s">
+      <c r="L20" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="M20" s="17" t="s">
+      <c r="M20" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="N20" s="17" t="s">
+      <c r="N20" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="O20" s="17" t="s">
+      <c r="O20" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P20" s="19" t="s">
+      <c r="P20" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="Q20" s="17" t="s">
+      <c r="Q20" s="4" t="s">
         <v>109</v>
       </c>
     </row>
@@ -5385,55 +5381,55 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="4">
         <v>12</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="18" t="s">
+      <c r="G24" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="H24" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="J24" s="17" t="s">
+      <c r="J24" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="K24" s="17" t="s">
+      <c r="K24" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="L24" s="17" t="s">
+      <c r="L24" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="M24" s="17" t="s">
+      <c r="M24" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="N24" s="17" t="s">
+      <c r="N24" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="O24" s="17" t="s">
+      <c r="O24" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P24" s="17" t="s">
+      <c r="P24" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="Q24" s="17" t="s">
+      <c r="Q24" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -5650,55 +5646,55 @@
       </c>
     </row>
     <row r="29" spans="1:17" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="4">
         <v>14</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G29" s="18" t="s">
+      <c r="G29" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="I29" s="17" t="s">
+      <c r="I29" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="J29" s="17" t="s">
+      <c r="J29" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="K29" s="17" t="s">
+      <c r="K29" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="L29" s="17" t="s">
+      <c r="L29" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="M29" s="22" t="s">
+      <c r="M29" s="18" t="s">
         <v>559</v>
       </c>
-      <c r="N29" s="17" t="s">
+      <c r="N29" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="O29" s="17" t="s">
+      <c r="O29" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P29" s="17" t="s">
+      <c r="P29" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="Q29" s="17" t="s">
+      <c r="Q29" s="4" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed layout of landing page, added react helmet, deleted timeline and projects pages
</commit_message>
<xml_diff>
--- a/src/recursos/BDD Timeline.xlsx
+++ b/src/recursos/BDD Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Files\Programming\portfolio\src\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD61A02-93EE-4975-B122-5E6C8955477D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281E54A1-F9D1-496D-9AE6-4FEC437DEA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
   </bookViews>
   <sheets>
     <sheet name="display" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="653">
   <si>
     <t>Location</t>
   </si>
@@ -6226,6 +6226,67 @@
 Las estrategias tácticas desempeñaron un papel vital en nuestro éxito en Raptors Gotcha. La lectura del campo nos permitió clasificar las rutas logísticas según su velocidad y previsibilidad. Esta comprensión nos permitió anticipar los movimientos y acciones del equipo contrario. Al analizar estratégicamente el campo, pudimos determinar las posiciones defensivas y planificar contraataques en consecuencia. La utilización adecuada del camuflaje, específicamente el patrón ATACS AU, nos ayudó a fundirnos perfectamente con el entorno semiárido. Sin embargo, aprendimos la importancia de planificar los movimientos a través de las sombras para evitar destacarnos involuntariamente en áreas iluminadas por el sol.*
 Los aspectos psicológicos de la sesión de entrenamiento enfatizaron la paciencia y el enfoque. Los enfrentamientos en campo verde requieren un constante cambio de atención entre el entorno, los compañeros de equipo y nuestros rifles de airsoft. Al mantener un flujo disciplinado y gestionar cuidadosamente nuestras acciones, mitigamos el riesgo de exponernos en campos abiertos o enfrentarnos a múltiples posiciones enemigas simultáneamente. Este enfoque deliberado, junto con la toma de decisiones estratégicas, nos permitió mantener una posición ventajosa durante todas las partidas.*
 En conclusión, la sesión de entrenamiento en Raptors Gotcha nos brindó conocimientos valiosos sobre la naturaleza compleja de las actividades de airsoft. La combinación de control físico, competencia táctica y resistencia psicológica resultó fundamental para superar los desafíos presentados por el terreno irregular y la vegetación densa del campo. Al aplicar los principios derivados del libro "La ciencia del entrenamiento de las artes marciales" de Charles I Staley, nuestro equipo de airsoft alcanzó un nivel superior de rendimiento y camaradería. En el futuro, continuaremos perfeccionando nuestras habilidades y tácticas, aprovechando las experiencias obtenidas de esta sesión de entrenamiento para destacar</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/1z2cyH27/RAPAX.png'</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/vTTvgXYq/aventureza.png</t>
+  </si>
+  <si>
+    <t>Aventureza</t>
+  </si>
+  <si>
+    <t>Software Engineer I</t>
+  </si>
+  <si>
+    <t>Ingeniero de software I</t>
+  </si>
+  <si>
+    <t>Somos un startup de capital mexicano conformado por un equipo de emprendedores apasionados con el desarrollo, crecimiento y digitalización de las industrias del entretenimiento, cultura y turismo en nuestro país y en América Latina.</t>
+  </si>
+  <si>
+    <t>We are a Mexican capital startup composed of a team of passionate entrepreneurs dedicated to the development, growth, and digitalization of the entertainment, culture, and tourism industries in our country and Latin America.</t>
+  </si>
+  <si>
+    <t>1) Mejorar las habilidades técnicas de un programador full stack que sea capaz de apoyar con el
+desarrollo frontend, backend o incluso de gestión de datos.
+2) Adquirir conocimientos teóricos en algoritmos, complejidad algorítmica en el tiempo, teoría de
+bases de datos relacionales, estructuras de datos básicos y avanzados, complejidad algorítmica
+en el espacio, Notación O,
+3) Desarrollar habilidades de administración del tiempo y proyectos con una especialización en
+proyectos de software que ayuden a calcular el tiempo necesario para completar tareas, dar
+seguimiento a resolución de problemas y comunicación efectiva con audiencias
+internas/externas de todos los niveles.
+4) Desarrollar e implementar pruebas automatizadas (unitarias, integración y E2E) usando el
+framework de JEST para las APIs backend que dan soporte a nuestras herramientas.
+5) Redactar, revisar y mantener los diagramas, guías y documentación de soporte relacionados a
+los proyectos de pagos, APIs backend y productos frontend
+6) Aprender a usar las tecnologías del stack de Aventureza a un nivel profesional. Estas están
+compuestas por: React-Native, Vue.js, Node.js, Jest.js, Serverless.com, AWS CLI, Javascript
+ES6/Typescript, BD PostgreSQL, BD NoSQL de Documentos, Web Tokens y Web Authentication,
+AWS Lambda, AWS API Gateway, AWS Cloudwatch, AWS Cognito, AWS SES, AWS IAM, AWS
+RDS, Firebase Developer tools, AWS Amplify.</t>
+  </si>
+  <si>
+    <t>Improve the technical skills of a full stack programmer who is capable of supporting frontend, backend, or even data management development.
+Acquire theoretical knowledge in algorithms, algorithmic complexity, relational database theory, basic and advanced data structures, algorithmic complexity in space, Big O notation.
+Develop time and project management skills with a specialization in software projects that help calculate the time needed to complete tasks, track problem resolution, and effectively communicate with internal/external audiences at all levels.
+Develop and implement automated tests (unit, integration, and end-to-end) using the JEST framework for backend APIs that support our tools.
+Write, review, and maintain diagrams, guides, and support documentation related to payment projects, backend APIs, and frontend products.
+Learn to use Aventureza's technology stack at a professional level. This stack includes: React-Native, Vue.js, Node.js, Jest.js, Serverless.com, AWS CLI, Javascript ES6/Typescript, PostgreSQL DB, NoSQL Document DB, Web Tokens and Web Authentication, AWS Lambda, AWS API Gateway, AWS Cloudwatch, AWS Cognito, AWS SES, AWS IAM, AWS RDS, Firebase Developer tools, AWS Amplify.</t>
+  </si>
+  <si>
+    <t>flexible</t>
+  </si>
+  <si>
+    <t>flex</t>
+  </si>
+  <si>
+    <t>sin definir</t>
+  </si>
+  <si>
+    <t>indefinido</t>
   </si>
 </sst>
 </file>
@@ -6412,11 +6473,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -7141,9 +7202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08630837-D9DA-4E92-997A-E80AD53DE965}">
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8521,8 +8580,8 @@
       <c r="A34" t="s">
         <v>243</v>
       </c>
-      <c r="B34" t="s">
-        <v>5</v>
+      <c r="B34" s="1" t="s">
+        <v>640</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>202</v>
@@ -8558,9 +8617,87 @@
         <v>393</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="I36" s="16"/>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>243</v>
+      </c>
+      <c r="B35" t="s">
+        <v>641</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D35" t="s">
+        <v>316</v>
+      </c>
+      <c r="E35" t="s">
+        <v>644</v>
+      </c>
+      <c r="F35" t="s">
+        <v>218</v>
+      </c>
+      <c r="G35" t="s">
+        <v>642</v>
+      </c>
+      <c r="H35" t="s">
+        <v>645</v>
+      </c>
+      <c r="I35" s="23" t="s">
+        <v>647</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>649</v>
+      </c>
+      <c r="K35" s="23" t="s">
+        <v>651</v>
+      </c>
+      <c r="L35" s="20">
+        <v>45084</v>
+      </c>
+      <c r="M35" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" t="s">
+        <v>641</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" t="s">
+        <v>643</v>
+      </c>
+      <c r="F36" t="s">
+        <v>218</v>
+      </c>
+      <c r="G36" t="s">
+        <v>642</v>
+      </c>
+      <c r="H36" t="s">
+        <v>646</v>
+      </c>
+      <c r="I36" s="23" t="s">
+        <v>648</v>
+      </c>
+      <c r="J36" s="23" t="s">
+        <v>650</v>
+      </c>
+      <c r="K36" s="23" t="s">
+        <v>652</v>
+      </c>
+      <c r="L36" s="20">
+        <v>45084</v>
+      </c>
+      <c r="M36" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
@@ -11493,8 +11630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774F871C-BEC6-4F34-9C8B-D56E8C7AB748}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11550,16 +11687,16 @@
       <c r="F2" t="s">
         <v>634</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" t="s">
         <v>626</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" t="s">
         <v>627</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="21" t="s">
         <v>629</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" t="s">
         <v>630</v>
       </c>
     </row>
@@ -11579,19 +11716,19 @@
       <c r="E3" t="s">
         <v>632</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>635</v>
       </c>
       <c r="G3" t="s">
         <v>636</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="22" t="s">
         <v>637</v>
       </c>
       <c r="I3" t="s">
         <v>638</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" t="s">
         <v>639</v>
       </c>
     </row>

</xml_diff>

<commit_message>
error fix y bloqueo de mantenimiento
</commit_message>
<xml_diff>
--- a/src/recursos/BDD Timeline.xlsx
+++ b/src/recursos/BDD Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Files\Programming\portfolio\src\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281E54A1-F9D1-496D-9AE6-4FEC437DEA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCDCA9A-F47B-4177-A6DA-32D280F0408D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{60294778-2A88-4BCF-91CA-79F00E7892F4}"/>
   </bookViews>
   <sheets>
     <sheet name="display" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="663">
   <si>
     <t>Location</t>
   </si>
@@ -3888,2238 +3888,6 @@
         <family val="3"/>
       </rPr>
       <t>handleChangeCatalog</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">.target.name, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.target.value)} /&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>  &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;Language:&lt;/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"Language"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{this.state.Language} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"text"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>onChange</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>{(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF9966B8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> this.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>handleChangeNotes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">.target.name, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.target.value)} /&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>  &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;Title:&lt;/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"Language"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{this.state.Language} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"text"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>onChange</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>{(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF9966B8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> this.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>handleChangeNotes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">.target.name, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.target.value)} /&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>  &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;Category:&lt;/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"Category"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{this.state.Category} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"text"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>onChange</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>{(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF9966B8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> this.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>handleChangeNotes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">.target.name, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.target.value)} /&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>  &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;HeaderImage:&lt;/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"HeaderImage"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{this.state.HeaderImage} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"text"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>onChange</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>{(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF9966B8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> this.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>handleChangeNotes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">.target.name, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.target.value)} /&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>  &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;SDescription:&lt;/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"SDescription"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{this.state.SDescription} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"text"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>onChange</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>{(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF9966B8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> this.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>handleChangeNotes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">.target.name, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.target.value)} /&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>  &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;Key:&lt;/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"Key"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{this.state.Key} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"text"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>onChange</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>{(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF9966B8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> this.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>handleChangeNotes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">.target.name, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.target.value)} /&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>  &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;Definition:&lt;/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"Definition"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{this.state.Definition} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"text"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>onChange</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>{(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF9966B8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> this.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>handleChangeNotes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">.target.name, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>.target.value)} /&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>  &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;Summary:&lt;/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>&gt;&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"Summary"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">{this.state.Summary} </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF22AA44"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>"text"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>onChange</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF225588"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>{(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF2277FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF9966B8"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>=&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF6688CC"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> this.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFDDBB88"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>handleChangeNotes</t>
     </r>
     <r>
       <rPr>
@@ -6287,6 +4055,60 @@
   </si>
   <si>
     <t>indefinido</t>
+  </si>
+  <si>
+    <t>Operación DEV-PRO</t>
+  </si>
+  <si>
+    <t>DEV-PRO Operation</t>
+  </si>
+  <si>
+    <t>Plan para otener empleo antes del cierre de año para los presupuestos basado en busquedas activas y capacitación continua</t>
+  </si>
+  <si>
+    <t>Plan to get a job before EOY for budget through continous training anc active searching</t>
+  </si>
+  <si>
+    <t>Buscar empleo como desarrollador junior en Ciudad de México antes de noviembre implica competir en un mercado laboral competitivo, adaptarse a opciones híbridas o remotas, y destacar entre la demanda alta, todo dentro de un plazo limitado.</t>
+  </si>
+  <si>
+    <t>Looking for a job as a junior developer en México City before november implies entering a competitive job market, adapting to hybrid or remote positions and standing out in high demand in a limited time schedule</t>
+  </si>
+  <si>
+    <t>Conseguir un trabajo en el cual desarrollar mi perfil y buscar futuras oportunidades de desarrollo</t>
+  </si>
+  <si>
+    <t>Start working in a job to develop my skill and profile for future development oportunities</t>
+  </si>
+  <si>
+    <t>Get a job by end of november</t>
+  </si>
+  <si>
+    <t>Conseguir empleo antes del fin de noviembre</t>
+  </si>
+  <si>
+    <t>7 semanas</t>
+  </si>
+  <si>
+    <t>7 weeks</t>
+  </si>
+  <si>
+    <t>["Evaluación y preparación", "Investigación de Mercado", "Apoyo externo", "Busqueda laboral", "Capacitación continua", "Documentación", "Ejecución del plan","Control y ajuste"]</t>
+  </si>
+  <si>
+    <t>["Analysis and training", "Market research", "External support", "Job hunt", "Continuos training", "Documentation", "Plan execution","Control and adjustments"]</t>
+  </si>
+  <si>
+    <t>1.- Portfolio, 2.- Lean enterprise tools, 3.- Project management tools, 4.- LinkedIn, 5.-NetworkAI by Wonsulting, 6.- Henry Job Board</t>
+  </si>
+  <si>
+    <t>in proceso</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1a3RpHW_6xYFxD-lIeNWfLKUWTjFw4AA-/edit?usp=sharing&amp;ouid=102349769484959538183&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t>1.- Portafolio, 2.- Herramientas de lean enterprise, 3.- Herramientas de administración de proyectos, 4.- LinkedIn, 5.-NetworkAI por Wonsulting, 6.- Henry Job Board</t>
   </si>
 </sst>
 </file>
@@ -6477,7 +4299,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -7202,7 +5024,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08630837-D9DA-4E92-997A-E80AD53DE965}">
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8581,7 +6405,7 @@
         <v>243</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>202</v>
@@ -8622,7 +6446,7 @@
         <v>243</v>
       </c>
       <c r="B35" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>200</v>
@@ -8631,25 +6455,25 @@
         <v>316</v>
       </c>
       <c r="E35" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="F35" t="s">
         <v>218</v>
       </c>
       <c r="G35" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="H35" t="s">
-        <v>645</v>
-      </c>
-      <c r="I35" s="23" t="s">
-        <v>647</v>
-      </c>
-      <c r="J35" s="23" t="s">
-        <v>649</v>
-      </c>
-      <c r="K35" s="23" t="s">
-        <v>651</v>
+        <v>637</v>
+      </c>
+      <c r="I35" t="s">
+        <v>639</v>
+      </c>
+      <c r="J35" t="s">
+        <v>641</v>
+      </c>
+      <c r="K35" t="s">
+        <v>643</v>
       </c>
       <c r="L35" s="20">
         <v>45084</v>
@@ -8663,7 +6487,7 @@
         <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>200</v>
@@ -8672,25 +6496,25 @@
         <v>47</v>
       </c>
       <c r="E36" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="F36" t="s">
         <v>218</v>
       </c>
       <c r="G36" t="s">
+        <v>634</v>
+      </c>
+      <c r="H36" t="s">
+        <v>638</v>
+      </c>
+      <c r="I36" t="s">
+        <v>640</v>
+      </c>
+      <c r="J36" t="s">
         <v>642</v>
       </c>
-      <c r="H36" t="s">
-        <v>646</v>
-      </c>
-      <c r="I36" s="23" t="s">
-        <v>648</v>
-      </c>
-      <c r="J36" s="23" t="s">
-        <v>650</v>
-      </c>
-      <c r="K36" s="23" t="s">
-        <v>652</v>
+      <c r="K36" t="s">
+        <v>644</v>
       </c>
       <c r="L36" s="20">
         <v>45084</v>
@@ -8803,11 +6627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACBE0D3-1FED-444E-85F3-AC56CB93C951}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Q10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q29" sqref="A29:Q29"/>
+    <sheetView topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10388,6 +8209,108 @@
       </c>
       <c r="Q29" s="4" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="4">
+        <v>15</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B31" s="4">
+        <v>15</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -10433,9 +8356,11 @@
     <hyperlink ref="G17" r:id="rId26" xr:uid="{3965A618-D2A1-4C20-AE39-9CA96872F9CF}"/>
     <hyperlink ref="G2" r:id="rId27" xr:uid="{72CAF257-10DA-4E0D-BB2E-DC56256F4B95}"/>
     <hyperlink ref="G5" r:id="rId28" xr:uid="{A76CAA92-FAD9-4B0A-BA85-B6A27F794D20}"/>
+    <hyperlink ref="G30" r:id="rId29" xr:uid="{23D83E89-1166-448D-871C-13B5547B24D9}"/>
+    <hyperlink ref="G31" r:id="rId30" xr:uid="{1B3AA55C-FFD9-47EC-B692-DB3E74DBA248}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
 
@@ -11470,8 +9395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BBBE35F-4D93-4FCA-A70E-C2AD585FB374}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11558,68 +9483,28 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>616</v>
-      </c>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>617</v>
-      </c>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>618</v>
-      </c>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>565</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>619</v>
-      </c>
+      <c r="C9" s="19"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>566</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>620</v>
-      </c>
+      <c r="C10" s="19"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>567</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>621</v>
-      </c>
+      <c r="C11" s="19"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>573</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>622</v>
-      </c>
+      <c r="C12" s="19"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>568</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>623</v>
-      </c>
+      <c r="C13" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11644,7 +9529,7 @@
         <v>178</v>
       </c>
       <c r="C1" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="D1" t="s">
         <v>45</v>
@@ -11662,7 +9547,7 @@
         <v>606</v>
       </c>
       <c r="I1" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="J1" t="s">
         <v>608</v>
@@ -11679,25 +9564,25 @@
         <v>45053</v>
       </c>
       <c r="D2" t="s">
+        <v>617</v>
+      </c>
+      <c r="E2" t="s">
         <v>625</v>
       </c>
-      <c r="E2" t="s">
-        <v>633</v>
-      </c>
       <c r="F2" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="G2" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="H2" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="J2" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
@@ -11711,25 +9596,25 @@
         <v>45053</v>
       </c>
       <c r="D3" t="s">
+        <v>623</v>
+      </c>
+      <c r="E3" t="s">
+        <v>624</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>627</v>
+      </c>
+      <c r="G3" t="s">
+        <v>628</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>629</v>
+      </c>
+      <c r="I3" t="s">
+        <v>630</v>
+      </c>
+      <c r="J3" t="s">
         <v>631</v>
-      </c>
-      <c r="E3" t="s">
-        <v>632</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>635</v>
-      </c>
-      <c r="G3" t="s">
-        <v>636</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>637</v>
-      </c>
-      <c r="I3" t="s">
-        <v>638</v>
-      </c>
-      <c r="J3" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>